<commit_message>
SCH - Pulse용 LED 추가, SWD용 Header 추가, XO 추가
</commit_message>
<xml_diff>
--- a/MCU PCB/Plasma_LF_MCU_PinMap_20180117.xlsx
+++ b/MCU PCB/Plasma_LF_MCU_PinMap_20180117.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12975" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12975"/>
   </bookViews>
   <sheets>
     <sheet name="Pin-map" sheetId="6" r:id="rId1"/>
@@ -14,7 +14,7 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Pin-map'!$B$15:$AB$79</definedName>
   </definedNames>
-  <calcPr calcId="144525"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
@@ -1950,7 +1950,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="14">
+  <fills count="15">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -2026,6 +2026,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0" tint="-0.34998626667073579"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2217,7 +2223,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="190">
+  <cellXfs count="193">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -2631,6 +2637,117 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="13" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="13" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="13" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="13" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="13" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="13" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="13" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="13" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="13" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="13" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="11" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="11" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -2649,116 +2766,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="11" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="5" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="11" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="13" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="13" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="13" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="13" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="13" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="13" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="13" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="13" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="13" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="13" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -2821,7 +2836,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -2856,7 +2871,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -3067,8 +3082,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:AB95"/>
   <sheetViews>
-    <sheetView topLeftCell="A70" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="Q85" sqref="Q85:R102"/>
+    <sheetView tabSelected="1" topLeftCell="F1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="U74" sqref="U74"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -3127,10 +3142,10 @@
       <c r="X2" s="1"/>
     </row>
     <row r="3" spans="2:27" x14ac:dyDescent="0.3">
-      <c r="B3" s="147" t="s">
+      <c r="B3" s="184" t="s">
         <v>3</v>
       </c>
-      <c r="C3" s="148"/>
+      <c r="C3" s="185"/>
       <c r="D3" s="2">
         <v>128</v>
       </c>
@@ -3158,10 +3173,10 @@
       </c>
     </row>
     <row r="4" spans="2:27" x14ac:dyDescent="0.3">
-      <c r="B4" s="149" t="s">
+      <c r="B4" s="186" t="s">
         <v>5</v>
       </c>
-      <c r="C4" s="150"/>
+      <c r="C4" s="187"/>
       <c r="D4" s="3">
         <v>16</v>
       </c>
@@ -3191,10 +3206,10 @@
       </c>
     </row>
     <row r="5" spans="2:27" x14ac:dyDescent="0.3">
-      <c r="B5" s="149" t="s">
+      <c r="B5" s="186" t="s">
         <v>6</v>
       </c>
-      <c r="C5" s="150"/>
+      <c r="C5" s="187"/>
       <c r="D5" s="3">
         <v>48</v>
       </c>
@@ -3226,10 +3241,10 @@
       </c>
     </row>
     <row r="6" spans="2:27" x14ac:dyDescent="0.3">
-      <c r="B6" s="149" t="s">
+      <c r="B6" s="186" t="s">
         <v>9</v>
       </c>
-      <c r="C6" s="150"/>
+      <c r="C6" s="187"/>
       <c r="D6" s="3" t="s">
         <v>10</v>
       </c>
@@ -3253,10 +3268,10 @@
       <c r="X6" s="18"/>
     </row>
     <row r="7" spans="2:27" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B7" s="151" t="s">
+      <c r="B7" s="188" t="s">
         <v>12</v>
       </c>
-      <c r="C7" s="152"/>
+      <c r="C7" s="189"/>
       <c r="D7" s="4" t="s">
         <v>13</v>
       </c>
@@ -3375,49 +3390,49 @@
     </row>
     <row r="13" spans="2:27" ht="17.25" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="14" spans="2:27" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B14" s="160" t="s">
+      <c r="B14" s="181" t="s">
         <v>178</v>
       </c>
-      <c r="C14" s="154"/>
-      <c r="D14" s="154" t="s">
+      <c r="C14" s="175"/>
+      <c r="D14" s="175" t="s">
         <v>163</v>
       </c>
-      <c r="E14" s="154" t="s">
+      <c r="E14" s="175" t="s">
         <v>165</v>
       </c>
-      <c r="F14" s="155"/>
-      <c r="G14" s="161" t="s">
+      <c r="F14" s="176"/>
+      <c r="G14" s="169" t="s">
         <v>14</v>
       </c>
-      <c r="H14" s="162"/>
-      <c r="I14" s="161" t="s">
+      <c r="H14" s="182"/>
+      <c r="I14" s="169" t="s">
         <v>311</v>
       </c>
-      <c r="J14" s="162"/>
-      <c r="K14" s="161" t="s">
+      <c r="J14" s="182"/>
+      <c r="K14" s="169" t="s">
         <v>312</v>
       </c>
-      <c r="L14" s="153"/>
+      <c r="L14" s="170"/>
       <c r="M14" s="23"/>
       <c r="N14" s="38"/>
-      <c r="O14" s="161" t="s">
+      <c r="O14" s="169" t="s">
         <v>14</v>
       </c>
-      <c r="P14" s="153"/>
-      <c r="Q14" s="153" t="s">
+      <c r="P14" s="170"/>
+      <c r="Q14" s="170" t="s">
         <v>162</v>
       </c>
-      <c r="R14" s="153"/>
+      <c r="R14" s="170"/>
       <c r="S14" s="58"/>
       <c r="T14" s="36"/>
-      <c r="V14" s="161" t="s">
+      <c r="V14" s="169" t="s">
         <v>14</v>
       </c>
-      <c r="W14" s="153"/>
-      <c r="X14" s="153" t="s">
+      <c r="W14" s="170"/>
+      <c r="X14" s="170" t="s">
         <v>383</v>
       </c>
-      <c r="Y14" s="153"/>
+      <c r="Y14" s="170"/>
       <c r="Z14" s="58"/>
       <c r="AA14" s="36"/>
     </row>
@@ -3428,7 +3443,7 @@
       <c r="C15" s="15" t="s">
         <v>180</v>
       </c>
-      <c r="D15" s="163"/>
+      <c r="D15" s="183"/>
       <c r="E15" s="15" t="s">
         <v>248</v>
       </c>
@@ -3506,10 +3521,10 @@
       <c r="D16" s="21" t="s">
         <v>164</v>
       </c>
-      <c r="E16" s="156" t="s">
+      <c r="E16" s="177" t="s">
         <v>176</v>
       </c>
-      <c r="F16" s="157"/>
+      <c r="F16" s="178"/>
       <c r="G16" s="52"/>
       <c r="H16" s="71"/>
       <c r="I16" s="81"/>
@@ -3642,22 +3657,22 @@
         <v>72</v>
       </c>
       <c r="T18" s="18"/>
-      <c r="V18" s="29" t="s">
-        <v>378</v>
-      </c>
-      <c r="W18" s="8" t="s">
+      <c r="V18" s="190" t="s">
+        <v>166</v>
+      </c>
+      <c r="W18" s="191" t="s">
         <v>379</v>
       </c>
-      <c r="X18" s="8" t="s">
-        <v>72</v>
-      </c>
-      <c r="Y18" s="8" t="s">
-        <v>72</v>
-      </c>
-      <c r="Z18" s="8" t="s">
-        <v>72</v>
-      </c>
-      <c r="AA18" s="18"/>
+      <c r="X18" s="191" t="s">
+        <v>72</v>
+      </c>
+      <c r="Y18" s="191" t="s">
+        <v>72</v>
+      </c>
+      <c r="Z18" s="191" t="s">
+        <v>72</v>
+      </c>
+      <c r="AA18" s="192"/>
     </row>
     <row r="19" spans="2:27" x14ac:dyDescent="0.3">
       <c r="B19" s="28">
@@ -3701,22 +3716,22 @@
         <v>72</v>
       </c>
       <c r="T19" s="18"/>
-      <c r="V19" s="29" t="s">
-        <v>378</v>
-      </c>
-      <c r="W19" s="8" t="s">
+      <c r="V19" s="190" t="s">
+        <v>167</v>
+      </c>
+      <c r="W19" s="191" t="s">
         <v>379</v>
       </c>
-      <c r="X19" s="8" t="s">
-        <v>72</v>
-      </c>
-      <c r="Y19" s="8" t="s">
-        <v>72</v>
-      </c>
-      <c r="Z19" s="8" t="s">
-        <v>72</v>
-      </c>
-      <c r="AA19" s="18"/>
+      <c r="X19" s="191" t="s">
+        <v>72</v>
+      </c>
+      <c r="Y19" s="191" t="s">
+        <v>72</v>
+      </c>
+      <c r="Z19" s="191" t="s">
+        <v>72</v>
+      </c>
+      <c r="AA19" s="192"/>
     </row>
     <row r="20" spans="2:27" x14ac:dyDescent="0.3">
       <c r="B20" s="28">
@@ -3758,22 +3773,22 @@
         <v>72</v>
       </c>
       <c r="T20" s="18"/>
-      <c r="V20" s="29" t="s">
-        <v>378</v>
-      </c>
-      <c r="W20" s="8" t="s">
+      <c r="V20" s="190" t="s">
+        <v>171</v>
+      </c>
+      <c r="W20" s="191" t="s">
         <v>379</v>
       </c>
-      <c r="X20" s="8" t="s">
-        <v>72</v>
-      </c>
-      <c r="Y20" s="8" t="s">
-        <v>72</v>
-      </c>
-      <c r="Z20" s="8" t="s">
-        <v>72</v>
-      </c>
-      <c r="AA20" s="18"/>
+      <c r="X20" s="191" t="s">
+        <v>72</v>
+      </c>
+      <c r="Y20" s="191" t="s">
+        <v>72</v>
+      </c>
+      <c r="Z20" s="191" t="s">
+        <v>72</v>
+      </c>
+      <c r="AA20" s="192"/>
     </row>
     <row r="21" spans="2:27" x14ac:dyDescent="0.3">
       <c r="B21" s="28">
@@ -3815,22 +3830,22 @@
         <v>72</v>
       </c>
       <c r="T21" s="18"/>
-      <c r="V21" s="29" t="s">
-        <v>378</v>
-      </c>
-      <c r="W21" s="8" t="s">
+      <c r="V21" s="190" t="s">
+        <v>175</v>
+      </c>
+      <c r="W21" s="191" t="s">
         <v>379</v>
       </c>
-      <c r="X21" s="8" t="s">
-        <v>72</v>
-      </c>
-      <c r="Y21" s="8" t="s">
-        <v>72</v>
-      </c>
-      <c r="Z21" s="8" t="s">
-        <v>72</v>
-      </c>
-      <c r="AA21" s="18"/>
+      <c r="X21" s="191" t="s">
+        <v>72</v>
+      </c>
+      <c r="Y21" s="191" t="s">
+        <v>72</v>
+      </c>
+      <c r="Z21" s="191" t="s">
+        <v>72</v>
+      </c>
+      <c r="AA21" s="192"/>
     </row>
     <row r="22" spans="2:27" x14ac:dyDescent="0.3">
       <c r="B22" s="28">
@@ -3842,10 +3857,10 @@
       <c r="D22" s="13" t="s">
         <v>170</v>
       </c>
-      <c r="E22" s="158" t="s">
+      <c r="E22" s="179" t="s">
         <v>177</v>
       </c>
-      <c r="F22" s="159"/>
+      <c r="F22" s="180"/>
       <c r="G22" s="66"/>
       <c r="H22" s="40"/>
       <c r="I22" s="29"/>
@@ -4169,10 +4184,10 @@
       <c r="D27" s="27" t="s">
         <v>187</v>
       </c>
-      <c r="E27" s="164" t="s">
+      <c r="E27" s="171" t="s">
         <v>189</v>
       </c>
-      <c r="F27" s="165"/>
+      <c r="F27" s="172"/>
       <c r="G27" s="67"/>
       <c r="H27" s="42"/>
       <c r="I27" s="29"/>
@@ -4204,10 +4219,10 @@
       <c r="D28" s="27" t="s">
         <v>188</v>
       </c>
-      <c r="E28" s="164" t="s">
+      <c r="E28" s="171" t="s">
         <v>190</v>
       </c>
-      <c r="F28" s="165"/>
+      <c r="F28" s="172"/>
       <c r="G28" s="67"/>
       <c r="H28" s="42"/>
       <c r="I28" s="29"/>
@@ -4475,10 +4490,10 @@
       <c r="D33" s="27" t="s">
         <v>219</v>
       </c>
-      <c r="E33" s="164" t="s">
+      <c r="E33" s="171" t="s">
         <v>195</v>
       </c>
-      <c r="F33" s="165"/>
+      <c r="F33" s="172"/>
       <c r="G33" s="67"/>
       <c r="H33" s="42"/>
       <c r="I33" s="29"/>
@@ -4510,10 +4525,10 @@
       <c r="D34" s="27" t="s">
         <v>164</v>
       </c>
-      <c r="E34" s="164" t="s">
+      <c r="E34" s="171" t="s">
         <v>176</v>
       </c>
-      <c r="F34" s="165"/>
+      <c r="F34" s="172"/>
       <c r="G34" s="67"/>
       <c r="H34" s="42"/>
       <c r="I34" s="29"/>
@@ -4733,19 +4748,19 @@
         <v>25</v>
       </c>
       <c r="T37" s="141"/>
-      <c r="V37" s="170" t="s">
+      <c r="V37" s="149" t="s">
         <v>102</v>
       </c>
-      <c r="W37" s="169" t="s">
+      <c r="W37" s="148" t="s">
         <v>22</v>
       </c>
-      <c r="X37" s="169" t="s">
+      <c r="X37" s="148" t="s">
         <v>103</v>
       </c>
-      <c r="Y37" s="169" t="s">
+      <c r="Y37" s="148" t="s">
         <v>104</v>
       </c>
-      <c r="Z37" s="169" t="s">
+      <c r="Z37" s="148" t="s">
         <v>25</v>
       </c>
       <c r="AA37" s="141"/>
@@ -4945,22 +4960,22 @@
       <c r="U40" s="1" t="s">
         <v>310</v>
       </c>
-      <c r="V40" s="171" t="s">
+      <c r="V40" s="150" t="s">
         <v>318</v>
       </c>
-      <c r="W40" s="172" t="s">
+      <c r="W40" s="151" t="s">
         <v>293</v>
       </c>
-      <c r="X40" s="172" t="s">
+      <c r="X40" s="151" t="s">
         <v>267</v>
       </c>
-      <c r="Y40" s="172" t="s">
+      <c r="Y40" s="151" t="s">
         <v>259</v>
       </c>
-      <c r="Z40" s="172" t="s">
+      <c r="Z40" s="151" t="s">
         <v>25</v>
       </c>
-      <c r="AA40" s="173"/>
+      <c r="AA40" s="152"/>
       <c r="AB40" s="1" t="s">
         <v>310</v>
       </c>
@@ -5019,22 +5034,22 @@
         <v>25</v>
       </c>
       <c r="T41" s="83"/>
-      <c r="V41" s="170" t="s">
+      <c r="V41" s="149" t="s">
         <v>21</v>
       </c>
-      <c r="W41" s="169" t="s">
+      <c r="W41" s="148" t="s">
         <v>22</v>
       </c>
-      <c r="X41" s="169" t="s">
+      <c r="X41" s="148" t="s">
         <v>258</v>
       </c>
-      <c r="Y41" s="169" t="s">
+      <c r="Y41" s="148" t="s">
         <v>268</v>
       </c>
-      <c r="Z41" s="169" t="s">
+      <c r="Z41" s="148" t="s">
         <v>25</v>
       </c>
-      <c r="AA41" s="173"/>
+      <c r="AA41" s="152"/>
     </row>
     <row r="42" spans="2:28" ht="33" x14ac:dyDescent="0.3">
       <c r="B42" s="28">
@@ -5093,20 +5108,20 @@
       <c r="U42" s="134" t="s">
         <v>380</v>
       </c>
-      <c r="V42" s="174" t="s">
+      <c r="V42" s="153" t="s">
         <v>313</v>
       </c>
-      <c r="W42" s="175" t="s">
+      <c r="W42" s="154" t="s">
         <v>22</v>
       </c>
-      <c r="X42" s="175" t="s">
+      <c r="X42" s="154" t="s">
         <v>315</v>
       </c>
-      <c r="Y42" s="175" t="s">
+      <c r="Y42" s="154" t="s">
         <v>290</v>
       </c>
-      <c r="Z42" s="175"/>
-      <c r="AA42" s="176" t="s">
+      <c r="Z42" s="154"/>
+      <c r="AA42" s="155" t="s">
         <v>275</v>
       </c>
       <c r="AB42" s="134" t="s">
@@ -5334,10 +5349,10 @@
       <c r="D46" s="27" t="s">
         <v>219</v>
       </c>
-      <c r="E46" s="164" t="s">
+      <c r="E46" s="171" t="s">
         <v>195</v>
       </c>
-      <c r="F46" s="165"/>
+      <c r="F46" s="172"/>
       <c r="G46" s="67"/>
       <c r="H46" s="42"/>
       <c r="I46" s="29"/>
@@ -5369,10 +5384,10 @@
       <c r="D47" s="27" t="s">
         <v>164</v>
       </c>
-      <c r="E47" s="164" t="s">
+      <c r="E47" s="171" t="s">
         <v>176</v>
       </c>
-      <c r="F47" s="165"/>
+      <c r="F47" s="172"/>
       <c r="G47" s="67"/>
       <c r="H47" s="42"/>
       <c r="I47" s="29"/>
@@ -5439,22 +5454,22 @@
       <c r="U48" s="1" t="s">
         <v>308</v>
       </c>
-      <c r="V48" s="170" t="s">
+      <c r="V48" s="149" t="s">
         <v>21</v>
       </c>
-      <c r="W48" s="169" t="s">
+      <c r="W48" s="148" t="s">
         <v>293</v>
       </c>
-      <c r="X48" s="169" t="s">
+      <c r="X48" s="148" t="s">
         <v>294</v>
       </c>
-      <c r="Y48" s="169" t="s">
+      <c r="Y48" s="148" t="s">
         <v>290</v>
       </c>
-      <c r="Z48" s="169" t="s">
+      <c r="Z48" s="148" t="s">
         <v>25</v>
       </c>
-      <c r="AA48" s="173"/>
+      <c r="AA48" s="152"/>
       <c r="AB48" s="1" t="s">
         <v>308</v>
       </c>
@@ -5636,22 +5651,22 @@
       <c r="U51" s="1" t="s">
         <v>309</v>
       </c>
-      <c r="V51" s="168" t="s">
+      <c r="V51" s="147" t="s">
         <v>275</v>
       </c>
-      <c r="W51" s="169" t="s">
+      <c r="W51" s="148" t="s">
         <v>22</v>
       </c>
-      <c r="X51" s="169" t="s">
+      <c r="X51" s="148" t="s">
         <v>289</v>
       </c>
-      <c r="Y51" s="169" t="s">
+      <c r="Y51" s="148" t="s">
         <v>272</v>
       </c>
-      <c r="Z51" s="169" t="s">
+      <c r="Z51" s="148" t="s">
         <v>25</v>
       </c>
-      <c r="AA51" s="173" t="s">
+      <c r="AA51" s="152" t="s">
         <v>304</v>
       </c>
       <c r="AB51" s="1" t="s">
@@ -5788,22 +5803,22 @@
       <c r="U53" s="1" t="s">
         <v>310</v>
       </c>
-      <c r="V53" s="171" t="s">
+      <c r="V53" s="150" t="s">
         <v>319</v>
       </c>
-      <c r="W53" s="172" t="s">
+      <c r="W53" s="151" t="s">
         <v>22</v>
       </c>
-      <c r="X53" s="172" t="s">
+      <c r="X53" s="151" t="s">
         <v>316</v>
       </c>
-      <c r="Y53" s="172" t="s">
+      <c r="Y53" s="151" t="s">
         <v>272</v>
       </c>
-      <c r="Z53" s="172" t="s">
+      <c r="Z53" s="151" t="s">
         <v>25</v>
       </c>
-      <c r="AA53" s="177" t="s">
+      <c r="AA53" s="156" t="s">
         <v>275</v>
       </c>
       <c r="AB53" s="1" t="s">
@@ -6262,22 +6277,22 @@
         <v>25</v>
       </c>
       <c r="T60" s="136"/>
-      <c r="V60" s="170" t="s">
+      <c r="V60" s="149" t="s">
         <v>21</v>
       </c>
-      <c r="W60" s="169" t="s">
+      <c r="W60" s="148" t="s">
         <v>293</v>
       </c>
-      <c r="X60" s="169" t="s">
+      <c r="X60" s="148" t="s">
         <v>279</v>
       </c>
-      <c r="Y60" s="169" t="s">
+      <c r="Y60" s="148" t="s">
         <v>250</v>
       </c>
-      <c r="Z60" s="169" t="s">
+      <c r="Z60" s="148" t="s">
         <v>25</v>
       </c>
-      <c r="AA60" s="173"/>
+      <c r="AA60" s="152"/>
     </row>
     <row r="61" spans="2:28" x14ac:dyDescent="0.3">
       <c r="B61" s="28">
@@ -6358,10 +6373,10 @@
       <c r="D62" s="27" t="s">
         <v>219</v>
       </c>
-      <c r="E62" s="164" t="s">
+      <c r="E62" s="171" t="s">
         <v>195</v>
       </c>
-      <c r="F62" s="165"/>
+      <c r="F62" s="172"/>
       <c r="G62" s="67"/>
       <c r="H62" s="42"/>
       <c r="I62" s="29"/>
@@ -6393,10 +6408,10 @@
       <c r="D63" s="27" t="s">
         <v>164</v>
       </c>
-      <c r="E63" s="164" t="s">
+      <c r="E63" s="171" t="s">
         <v>176</v>
       </c>
-      <c r="F63" s="165"/>
+      <c r="F63" s="172"/>
       <c r="G63" s="67"/>
       <c r="H63" s="42"/>
       <c r="I63" s="29"/>
@@ -7189,10 +7204,10 @@
       <c r="D75" s="51" t="s">
         <v>225</v>
       </c>
-      <c r="E75" s="164" t="s">
+      <c r="E75" s="171" t="s">
         <v>244</v>
       </c>
-      <c r="F75" s="165"/>
+      <c r="F75" s="172"/>
       <c r="G75" s="67"/>
       <c r="H75" s="65"/>
       <c r="I75" s="30"/>
@@ -7390,10 +7405,10 @@
       <c r="D78" s="27" t="s">
         <v>219</v>
       </c>
-      <c r="E78" s="164" t="s">
+      <c r="E78" s="171" t="s">
         <v>195</v>
       </c>
-      <c r="F78" s="165"/>
+      <c r="F78" s="172"/>
       <c r="G78" s="67"/>
       <c r="H78" s="42"/>
       <c r="I78" s="29"/>
@@ -7425,10 +7440,10 @@
       <c r="D79" s="32" t="s">
         <v>164</v>
       </c>
-      <c r="E79" s="166" t="s">
+      <c r="E79" s="173" t="s">
         <v>176</v>
       </c>
-      <c r="F79" s="167"/>
+      <c r="F79" s="174"/>
       <c r="G79" s="68"/>
       <c r="H79" s="70"/>
       <c r="I79" s="75"/>
@@ -7501,11 +7516,16 @@
   </sheetData>
   <autoFilter ref="B15:AB79"/>
   <mergeCells count="28">
-    <mergeCell ref="V14:W14"/>
-    <mergeCell ref="X14:Y14"/>
-    <mergeCell ref="E47:F47"/>
-    <mergeCell ref="E62:F62"/>
-    <mergeCell ref="E63:F63"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="B4:C4"/>
+    <mergeCell ref="B5:C5"/>
+    <mergeCell ref="B6:C6"/>
+    <mergeCell ref="B7:C7"/>
+    <mergeCell ref="B14:C14"/>
+    <mergeCell ref="I14:J14"/>
+    <mergeCell ref="K14:L14"/>
+    <mergeCell ref="D14:D15"/>
+    <mergeCell ref="G14:H14"/>
     <mergeCell ref="E78:F78"/>
     <mergeCell ref="E79:F79"/>
     <mergeCell ref="E75:F75"/>
@@ -7514,21 +7534,16 @@
     <mergeCell ref="E33:F33"/>
     <mergeCell ref="E34:F34"/>
     <mergeCell ref="E46:F46"/>
+    <mergeCell ref="V14:W14"/>
+    <mergeCell ref="X14:Y14"/>
+    <mergeCell ref="E47:F47"/>
+    <mergeCell ref="E62:F62"/>
+    <mergeCell ref="E63:F63"/>
     <mergeCell ref="Q14:R14"/>
     <mergeCell ref="E14:F14"/>
     <mergeCell ref="E16:F16"/>
     <mergeCell ref="E22:F22"/>
-    <mergeCell ref="B14:C14"/>
-    <mergeCell ref="I14:J14"/>
-    <mergeCell ref="K14:L14"/>
-    <mergeCell ref="D14:D15"/>
-    <mergeCell ref="G14:H14"/>
     <mergeCell ref="O14:P14"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="B4:C4"/>
-    <mergeCell ref="B5:C5"/>
-    <mergeCell ref="B6:C6"/>
-    <mergeCell ref="B7:C7"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -8185,29 +8200,29 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:N46"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="Q17" sqref="Q17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="9" style="179"/>
-    <col min="3" max="3" width="12.75" style="178" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.625" style="178" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.625" style="178" customWidth="1"/>
-    <col min="6" max="6" width="9" style="179"/>
-    <col min="7" max="7" width="11.875" style="178" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="11.375" style="178" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9" style="158"/>
+    <col min="3" max="3" width="12.75" style="157" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.625" style="157" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.625" style="157" customWidth="1"/>
+    <col min="6" max="6" width="9" style="158"/>
+    <col min="7" max="7" width="11.875" style="157" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.375" style="157" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="11.375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:14" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B2" s="179" t="s">
+      <c r="B2" s="158" t="s">
         <v>421</v>
       </c>
     </row>
-    <row r="3" spans="2:14" s="179" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="180" t="s">
+    <row r="3" spans="2:14" s="158" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B3" s="159" t="s">
         <v>459</v>
       </c>
       <c r="C3" s="120" t="s">
@@ -8219,7 +8234,7 @@
       <c r="E3" s="121" t="s">
         <v>464</v>
       </c>
-      <c r="F3" s="180" t="s">
+      <c r="F3" s="159" t="s">
         <v>459</v>
       </c>
       <c r="G3" s="120" t="s">
@@ -8233,23 +8248,23 @@
       </c>
     </row>
     <row r="4" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B4" s="188">
+      <c r="B4" s="167">
         <v>1</v>
       </c>
-      <c r="C4" s="186" t="s">
+      <c r="C4" s="165" t="s">
         <v>384</v>
       </c>
-      <c r="D4" s="181" t="s">
+      <c r="D4" s="160" t="s">
         <v>444</v>
       </c>
-      <c r="E4" s="182"/>
-      <c r="F4" s="188">
+      <c r="E4" s="161"/>
+      <c r="F4" s="167">
         <v>2</v>
       </c>
-      <c r="G4" s="186" t="s">
+      <c r="G4" s="165" t="s">
         <v>385</v>
       </c>
-      <c r="H4" s="181" t="s">
+      <c r="H4" s="160" t="s">
         <v>444</v>
       </c>
       <c r="I4" s="117"/>
@@ -8261,25 +8276,25 @@
       </c>
     </row>
     <row r="5" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B5" s="188">
+      <c r="B5" s="167">
         <v>3</v>
       </c>
-      <c r="C5" s="186" t="s">
+      <c r="C5" s="165" t="s">
         <v>386</v>
       </c>
-      <c r="D5" s="186" t="s">
+      <c r="D5" s="165" t="s">
         <v>445</v>
       </c>
-      <c r="E5" s="185" t="s">
+      <c r="E5" s="164" t="s">
         <v>454</v>
       </c>
-      <c r="F5" s="188">
+      <c r="F5" s="167">
         <v>4</v>
       </c>
-      <c r="G5" s="186" t="s">
+      <c r="G5" s="165" t="s">
         <v>387</v>
       </c>
-      <c r="H5" s="181" t="s">
+      <c r="H5" s="160" t="s">
         <v>444</v>
       </c>
       <c r="I5" s="117"/>
@@ -8291,23 +8306,23 @@
       </c>
     </row>
     <row r="6" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B6" s="188">
+      <c r="B6" s="167">
         <v>5</v>
       </c>
-      <c r="C6" s="186" t="s">
+      <c r="C6" s="165" t="s">
         <v>388</v>
       </c>
-      <c r="D6" s="186" t="s">
+      <c r="D6" s="165" t="s">
         <v>446</v>
       </c>
-      <c r="E6" s="185"/>
-      <c r="F6" s="188">
+      <c r="E6" s="164"/>
+      <c r="F6" s="167">
         <v>6</v>
       </c>
-      <c r="G6" s="186" t="s">
+      <c r="G6" s="165" t="s">
         <v>389</v>
       </c>
-      <c r="H6" s="181" t="s">
+      <c r="H6" s="160" t="s">
         <v>444</v>
       </c>
       <c r="I6" s="117"/>
@@ -8321,23 +8336,23 @@
       </c>
     </row>
     <row r="7" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B7" s="188">
+      <c r="B7" s="167">
         <v>7</v>
       </c>
-      <c r="C7" s="186" t="s">
+      <c r="C7" s="165" t="s">
         <v>390</v>
       </c>
-      <c r="D7" s="186" t="s">
+      <c r="D7" s="165" t="s">
         <v>447</v>
       </c>
-      <c r="E7" s="185"/>
-      <c r="F7" s="188">
+      <c r="E7" s="164"/>
+      <c r="F7" s="167">
         <v>8</v>
       </c>
-      <c r="G7" s="186" t="s">
+      <c r="G7" s="165" t="s">
         <v>392</v>
       </c>
-      <c r="H7" s="181" t="s">
+      <c r="H7" s="160" t="s">
         <v>444</v>
       </c>
       <c r="I7" s="117"/>
@@ -8349,23 +8364,23 @@
       </c>
     </row>
     <row r="8" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B8" s="188">
+      <c r="B8" s="167">
         <v>9</v>
       </c>
-      <c r="C8" s="186" t="s">
+      <c r="C8" s="165" t="s">
         <v>391</v>
       </c>
-      <c r="D8" s="181" t="s">
+      <c r="D8" s="160" t="s">
         <v>444</v>
       </c>
-      <c r="E8" s="182"/>
-      <c r="F8" s="188">
+      <c r="E8" s="161"/>
+      <c r="F8" s="167">
         <v>10</v>
       </c>
-      <c r="G8" s="186" t="s">
+      <c r="G8" s="165" t="s">
         <v>393</v>
       </c>
-      <c r="H8" s="181" t="s">
+      <c r="H8" s="160" t="s">
         <v>444</v>
       </c>
       <c r="I8" s="117"/>
@@ -8379,23 +8394,23 @@
       </c>
     </row>
     <row r="9" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B9" s="188">
+      <c r="B9" s="167">
         <v>11</v>
       </c>
-      <c r="C9" s="186" t="s">
+      <c r="C9" s="165" t="s">
         <v>394</v>
       </c>
-      <c r="D9" s="181" t="s">
+      <c r="D9" s="160" t="s">
         <v>444</v>
       </c>
-      <c r="E9" s="182"/>
-      <c r="F9" s="188">
+      <c r="E9" s="161"/>
+      <c r="F9" s="167">
         <v>12</v>
       </c>
-      <c r="G9" s="186" t="s">
+      <c r="G9" s="165" t="s">
         <v>395</v>
       </c>
-      <c r="H9" s="181" t="s">
+      <c r="H9" s="160" t="s">
         <v>444</v>
       </c>
       <c r="I9" s="117"/>
@@ -8408,23 +8423,23 @@
       </c>
     </row>
     <row r="10" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B10" s="188">
+      <c r="B10" s="167">
         <v>13</v>
       </c>
-      <c r="C10" s="186" t="s">
+      <c r="C10" s="165" t="s">
         <v>396</v>
       </c>
-      <c r="D10" s="181" t="s">
+      <c r="D10" s="160" t="s">
         <v>444</v>
       </c>
-      <c r="E10" s="182"/>
-      <c r="F10" s="188">
+      <c r="E10" s="161"/>
+      <c r="F10" s="167">
         <v>14</v>
       </c>
-      <c r="G10" s="186" t="s">
+      <c r="G10" s="165" t="s">
         <v>397</v>
       </c>
-      <c r="H10" s="181" t="s">
+      <c r="H10" s="160" t="s">
         <v>444</v>
       </c>
       <c r="I10" s="117"/>
@@ -8435,23 +8450,23 @@
       <c r="N10" s="5"/>
     </row>
     <row r="11" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B11" s="188">
+      <c r="B11" s="167">
         <v>15</v>
       </c>
-      <c r="C11" s="186" t="s">
+      <c r="C11" s="165" t="s">
         <v>398</v>
       </c>
-      <c r="D11" s="181" t="s">
+      <c r="D11" s="160" t="s">
         <v>444</v>
       </c>
-      <c r="E11" s="182"/>
-      <c r="F11" s="188">
+      <c r="E11" s="161"/>
+      <c r="F11" s="167">
         <v>16</v>
       </c>
-      <c r="G11" s="186" t="s">
+      <c r="G11" s="165" t="s">
         <v>400</v>
       </c>
-      <c r="H11" s="181" t="s">
+      <c r="H11" s="160" t="s">
         <v>444</v>
       </c>
       <c r="I11" s="117"/>
@@ -8462,23 +8477,23 @@
       <c r="N11" s="5"/>
     </row>
     <row r="12" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B12" s="188">
+      <c r="B12" s="167">
         <v>17</v>
       </c>
-      <c r="C12" s="186" t="s">
+      <c r="C12" s="165" t="s">
         <v>399</v>
       </c>
-      <c r="D12" s="181" t="s">
+      <c r="D12" s="160" t="s">
         <v>444</v>
       </c>
-      <c r="E12" s="182"/>
-      <c r="F12" s="188">
+      <c r="E12" s="161"/>
+      <c r="F12" s="167">
         <v>18</v>
       </c>
-      <c r="G12" s="186" t="s">
+      <c r="G12" s="165" t="s">
         <v>401</v>
       </c>
-      <c r="H12" s="181" t="s">
+      <c r="H12" s="160" t="s">
         <v>444</v>
       </c>
       <c r="I12" s="117"/>
@@ -8486,23 +8501,23 @@
       <c r="N12" s="5"/>
     </row>
     <row r="13" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B13" s="188">
+      <c r="B13" s="167">
         <v>19</v>
       </c>
-      <c r="C13" s="186" t="s">
+      <c r="C13" s="165" t="s">
         <v>402</v>
       </c>
-      <c r="D13" s="186" t="s">
+      <c r="D13" s="165" t="s">
         <v>402</v>
       </c>
-      <c r="E13" s="185"/>
-      <c r="F13" s="188">
+      <c r="E13" s="164"/>
+      <c r="F13" s="167">
         <v>20</v>
       </c>
-      <c r="G13" s="186" t="s">
+      <c r="G13" s="165" t="s">
         <v>403</v>
       </c>
-      <c r="H13" s="186" t="s">
+      <c r="H13" s="165" t="s">
         <v>403</v>
       </c>
       <c r="I13" s="117"/>
@@ -8510,23 +8525,23 @@
       <c r="N13" s="5"/>
     </row>
     <row r="14" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B14" s="188">
+      <c r="B14" s="167">
         <v>21</v>
       </c>
-      <c r="C14" s="186" t="s">
+      <c r="C14" s="165" t="s">
         <v>404</v>
       </c>
-      <c r="D14" s="186" t="s">
+      <c r="D14" s="165" t="s">
         <v>448</v>
       </c>
-      <c r="E14" s="185"/>
-      <c r="F14" s="188">
+      <c r="E14" s="164"/>
+      <c r="F14" s="167">
         <v>22</v>
       </c>
-      <c r="G14" s="186" t="s">
+      <c r="G14" s="165" t="s">
         <v>405</v>
       </c>
-      <c r="H14" s="181" t="s">
+      <c r="H14" s="160" t="s">
         <v>444</v>
       </c>
       <c r="I14" s="117"/>
@@ -8536,23 +8551,23 @@
       <c r="N14" s="5"/>
     </row>
     <row r="15" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B15" s="188">
+      <c r="B15" s="167">
         <v>23</v>
       </c>
-      <c r="C15" s="186" t="s">
+      <c r="C15" s="165" t="s">
         <v>406</v>
       </c>
-      <c r="D15" s="186" t="s">
+      <c r="D15" s="165" t="s">
         <v>448</v>
       </c>
-      <c r="E15" s="185"/>
-      <c r="F15" s="188">
+      <c r="E15" s="164"/>
+      <c r="F15" s="167">
         <v>24</v>
       </c>
-      <c r="G15" s="186" t="s">
+      <c r="G15" s="165" t="s">
         <v>406</v>
       </c>
-      <c r="H15" s="181" t="s">
+      <c r="H15" s="160" t="s">
         <v>444</v>
       </c>
       <c r="I15" s="117"/>
@@ -8562,23 +8577,23 @@
       <c r="N15" s="5"/>
     </row>
     <row r="16" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B16" s="188">
+      <c r="B16" s="167">
         <v>25</v>
       </c>
-      <c r="C16" s="186" t="s">
+      <c r="C16" s="165" t="s">
         <v>407</v>
       </c>
-      <c r="D16" s="181" t="s">
+      <c r="D16" s="160" t="s">
         <v>444</v>
       </c>
-      <c r="E16" s="182"/>
-      <c r="F16" s="188">
+      <c r="E16" s="161"/>
+      <c r="F16" s="167">
         <v>26</v>
       </c>
-      <c r="G16" s="186" t="s">
+      <c r="G16" s="165" t="s">
         <v>414</v>
       </c>
-      <c r="H16" s="181" t="s">
+      <c r="H16" s="160" t="s">
         <v>444</v>
       </c>
       <c r="I16" s="117"/>
@@ -8589,23 +8604,23 @@
       <c r="N16" s="5"/>
     </row>
     <row r="17" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B17" s="188">
+      <c r="B17" s="167">
         <v>27</v>
       </c>
-      <c r="C17" s="186" t="s">
+      <c r="C17" s="165" t="s">
         <v>408</v>
       </c>
-      <c r="D17" s="181" t="s">
+      <c r="D17" s="160" t="s">
         <v>444</v>
       </c>
-      <c r="E17" s="182"/>
-      <c r="F17" s="188">
+      <c r="E17" s="161"/>
+      <c r="F17" s="167">
         <v>28</v>
       </c>
-      <c r="G17" s="186" t="s">
+      <c r="G17" s="165" t="s">
         <v>415</v>
       </c>
-      <c r="H17" s="181" t="s">
+      <c r="H17" s="160" t="s">
         <v>444</v>
       </c>
       <c r="I17" s="117"/>
@@ -8613,23 +8628,23 @@
       <c r="N17" s="5"/>
     </row>
     <row r="18" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B18" s="188">
+      <c r="B18" s="167">
         <v>29</v>
       </c>
-      <c r="C18" s="186" t="s">
+      <c r="C18" s="165" t="s">
         <v>409</v>
       </c>
-      <c r="D18" s="181" t="s">
+      <c r="D18" s="160" t="s">
         <v>444</v>
       </c>
-      <c r="E18" s="182"/>
-      <c r="F18" s="188">
+      <c r="E18" s="161"/>
+      <c r="F18" s="167">
         <v>30</v>
       </c>
-      <c r="G18" s="186" t="s">
+      <c r="G18" s="165" t="s">
         <v>416</v>
       </c>
-      <c r="H18" s="181" t="s">
+      <c r="H18" s="160" t="s">
         <v>444</v>
       </c>
       <c r="I18" s="117"/>
@@ -8637,23 +8652,23 @@
       <c r="N18" s="5"/>
     </row>
     <row r="19" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B19" s="188">
+      <c r="B19" s="167">
         <v>31</v>
       </c>
-      <c r="C19" s="186" t="s">
+      <c r="C19" s="165" t="s">
         <v>410</v>
       </c>
-      <c r="D19" s="181" t="s">
+      <c r="D19" s="160" t="s">
         <v>444</v>
       </c>
-      <c r="E19" s="182"/>
-      <c r="F19" s="188">
+      <c r="E19" s="161"/>
+      <c r="F19" s="167">
         <v>32</v>
       </c>
-      <c r="G19" s="186" t="s">
+      <c r="G19" s="165" t="s">
         <v>417</v>
       </c>
-      <c r="H19" s="181" t="s">
+      <c r="H19" s="160" t="s">
         <v>444</v>
       </c>
       <c r="I19" s="117"/>
@@ -8661,23 +8676,23 @@
       <c r="N19" s="5"/>
     </row>
     <row r="20" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B20" s="188">
+      <c r="B20" s="167">
         <v>33</v>
       </c>
-      <c r="C20" s="186" t="s">
+      <c r="C20" s="165" t="s">
         <v>411</v>
       </c>
-      <c r="D20" s="181" t="s">
+      <c r="D20" s="160" t="s">
         <v>444</v>
       </c>
-      <c r="E20" s="182"/>
-      <c r="F20" s="188">
+      <c r="E20" s="161"/>
+      <c r="F20" s="167">
         <v>34</v>
       </c>
-      <c r="G20" s="186" t="s">
+      <c r="G20" s="165" t="s">
         <v>418</v>
       </c>
-      <c r="H20" s="181" t="s">
+      <c r="H20" s="160" t="s">
         <v>444</v>
       </c>
       <c r="I20" s="117"/>
@@ -8687,23 +8702,23 @@
       <c r="N20" s="5"/>
     </row>
     <row r="21" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B21" s="188">
+      <c r="B21" s="167">
         <v>35</v>
       </c>
-      <c r="C21" s="186" t="s">
+      <c r="C21" s="165" t="s">
         <v>412</v>
       </c>
-      <c r="D21" s="181" t="s">
+      <c r="D21" s="160" t="s">
         <v>444</v>
       </c>
-      <c r="E21" s="182"/>
-      <c r="F21" s="188">
+      <c r="E21" s="161"/>
+      <c r="F21" s="167">
         <v>36</v>
       </c>
-      <c r="G21" s="186" t="s">
+      <c r="G21" s="165" t="s">
         <v>419</v>
       </c>
-      <c r="H21" s="181" t="s">
+      <c r="H21" s="160" t="s">
         <v>444</v>
       </c>
       <c r="I21" s="117"/>
@@ -8713,23 +8728,23 @@
       <c r="N21" s="5"/>
     </row>
     <row r="22" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B22" s="188">
+      <c r="B22" s="167">
         <v>37</v>
       </c>
-      <c r="C22" s="186" t="s">
+      <c r="C22" s="165" t="s">
         <v>413</v>
       </c>
-      <c r="D22" s="181" t="s">
+      <c r="D22" s="160" t="s">
         <v>444</v>
       </c>
-      <c r="E22" s="182"/>
-      <c r="F22" s="188">
+      <c r="E22" s="161"/>
+      <c r="F22" s="167">
         <v>38</v>
       </c>
-      <c r="G22" s="186" t="s">
+      <c r="G22" s="165" t="s">
         <v>420</v>
       </c>
-      <c r="H22" s="181" t="s">
+      <c r="H22" s="160" t="s">
         <v>444</v>
       </c>
       <c r="I22" s="117"/>
@@ -8739,34 +8754,34 @@
       </c>
     </row>
     <row r="23" spans="2:14" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B23" s="189">
+      <c r="B23" s="168">
         <v>39</v>
       </c>
-      <c r="C23" s="187" t="s">
+      <c r="C23" s="166" t="s">
         <v>408</v>
       </c>
-      <c r="D23" s="183" t="s">
+      <c r="D23" s="162" t="s">
         <v>444</v>
       </c>
-      <c r="E23" s="184"/>
-      <c r="F23" s="189">
+      <c r="E23" s="163"/>
+      <c r="F23" s="168">
         <v>40</v>
       </c>
-      <c r="G23" s="187" t="s">
+      <c r="G23" s="166" t="s">
         <v>415</v>
       </c>
-      <c r="H23" s="183" t="s">
+      <c r="H23" s="162" t="s">
         <v>444</v>
       </c>
       <c r="I23" s="119"/>
     </row>
     <row r="25" spans="2:14" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B25" s="179" t="s">
+      <c r="B25" s="158" t="s">
         <v>422</v>
       </c>
     </row>
-    <row r="26" spans="2:14" s="179" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="B26" s="180" t="s">
+    <row r="26" spans="2:14" s="158" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B26" s="159" t="s">
         <v>459</v>
       </c>
       <c r="C26" s="120" t="s">
@@ -8778,7 +8793,7 @@
       <c r="E26" s="121" t="s">
         <v>464</v>
       </c>
-      <c r="F26" s="180" t="s">
+      <c r="F26" s="159" t="s">
         <v>459</v>
       </c>
       <c r="G26" s="120" t="s">
@@ -8792,451 +8807,451 @@
       </c>
     </row>
     <row r="27" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B27" s="188">
+      <c r="B27" s="167">
         <v>1</v>
       </c>
-      <c r="C27" s="186" t="s">
+      <c r="C27" s="165" t="s">
         <v>455</v>
       </c>
-      <c r="D27" s="186" t="s">
+      <c r="D27" s="165" t="s">
         <v>449</v>
       </c>
-      <c r="E27" s="185" t="s">
+      <c r="E27" s="164" t="s">
         <v>460</v>
       </c>
-      <c r="F27" s="188">
+      <c r="F27" s="167">
         <v>2</v>
       </c>
-      <c r="G27" s="186" t="s">
+      <c r="G27" s="165" t="s">
         <v>426</v>
       </c>
-      <c r="H27" s="181" t="s">
+      <c r="H27" s="160" t="s">
         <v>444</v>
       </c>
       <c r="I27" s="117"/>
     </row>
     <row r="28" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B28" s="188">
+      <c r="B28" s="167">
         <v>3</v>
       </c>
-      <c r="C28" s="186" t="s">
+      <c r="C28" s="165" t="s">
         <v>425</v>
       </c>
-      <c r="D28" s="181" t="s">
+      <c r="D28" s="160" t="s">
         <v>444</v>
       </c>
-      <c r="E28" s="182"/>
-      <c r="F28" s="188">
+      <c r="E28" s="161"/>
+      <c r="F28" s="167">
         <v>4</v>
       </c>
-      <c r="G28" s="186" t="s">
+      <c r="G28" s="165" t="s">
         <v>427</v>
       </c>
-      <c r="H28" s="181" t="s">
+      <c r="H28" s="160" t="s">
         <v>444</v>
       </c>
       <c r="I28" s="117"/>
     </row>
     <row r="29" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B29" s="188">
+      <c r="B29" s="167">
         <v>5</v>
       </c>
-      <c r="C29" s="186" t="s">
+      <c r="C29" s="165" t="s">
         <v>423</v>
       </c>
-      <c r="D29" s="181" t="s">
+      <c r="D29" s="160" t="s">
         <v>444</v>
       </c>
-      <c r="E29" s="182"/>
-      <c r="F29" s="188">
+      <c r="E29" s="161"/>
+      <c r="F29" s="167">
         <v>6</v>
       </c>
-      <c r="G29" s="186" t="s">
+      <c r="G29" s="165" t="s">
         <v>428</v>
       </c>
-      <c r="H29" s="181" t="s">
+      <c r="H29" s="160" t="s">
         <v>444</v>
       </c>
       <c r="I29" s="117"/>
     </row>
     <row r="30" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B30" s="188">
+      <c r="B30" s="167">
         <v>7</v>
       </c>
-      <c r="C30" s="186" t="s">
+      <c r="C30" s="165" t="s">
         <v>424</v>
       </c>
-      <c r="D30" s="181" t="s">
+      <c r="D30" s="160" t="s">
         <v>444</v>
       </c>
-      <c r="E30" s="182"/>
-      <c r="F30" s="188">
+      <c r="E30" s="161"/>
+      <c r="F30" s="167">
         <v>8</v>
       </c>
-      <c r="G30" s="186" t="s">
+      <c r="G30" s="165" t="s">
         <v>425</v>
       </c>
-      <c r="H30" s="181" t="s">
+      <c r="H30" s="160" t="s">
         <v>444</v>
       </c>
       <c r="I30" s="117"/>
     </row>
     <row r="31" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B31" s="188">
+      <c r="B31" s="167">
         <v>9</v>
       </c>
-      <c r="C31" s="186" t="s">
+      <c r="C31" s="165" t="s">
         <v>404</v>
       </c>
-      <c r="D31" s="181" t="s">
+      <c r="D31" s="160" t="s">
         <v>444</v>
       </c>
-      <c r="E31" s="182"/>
-      <c r="F31" s="188">
+      <c r="E31" s="161"/>
+      <c r="F31" s="167">
         <v>10</v>
       </c>
-      <c r="G31" s="186" t="s">
+      <c r="G31" s="165" t="s">
         <v>405</v>
       </c>
-      <c r="H31" s="181" t="s">
+      <c r="H31" s="160" t="s">
         <v>444</v>
       </c>
       <c r="I31" s="117"/>
     </row>
     <row r="32" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B32" s="188">
+      <c r="B32" s="167">
         <v>11</v>
       </c>
-      <c r="C32" s="186" t="s">
+      <c r="C32" s="165" t="s">
         <v>429</v>
       </c>
-      <c r="D32" s="181" t="s">
+      <c r="D32" s="160" t="s">
         <v>444</v>
       </c>
-      <c r="E32" s="182"/>
-      <c r="F32" s="188">
+      <c r="E32" s="161"/>
+      <c r="F32" s="167">
         <v>12</v>
       </c>
-      <c r="G32" s="186" t="s">
+      <c r="G32" s="165" t="s">
         <v>438</v>
       </c>
-      <c r="H32" s="181" t="s">
+      <c r="H32" s="160" t="s">
         <v>444</v>
       </c>
       <c r="I32" s="117"/>
     </row>
     <row r="33" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B33" s="188">
+      <c r="B33" s="167">
         <v>13</v>
       </c>
-      <c r="C33" s="186" t="s">
+      <c r="C33" s="165" t="s">
         <v>456</v>
       </c>
-      <c r="D33" s="186" t="s">
+      <c r="D33" s="165" t="s">
         <v>450</v>
       </c>
-      <c r="E33" s="185" t="s">
+      <c r="E33" s="164" t="s">
         <v>461</v>
       </c>
-      <c r="F33" s="188">
+      <c r="F33" s="167">
         <v>14</v>
       </c>
-      <c r="G33" s="186" t="s">
+      <c r="G33" s="165" t="s">
         <v>411</v>
       </c>
-      <c r="H33" s="181" t="s">
+      <c r="H33" s="160" t="s">
         <v>444</v>
       </c>
       <c r="I33" s="117"/>
     </row>
     <row r="34" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B34" s="188">
+      <c r="B34" s="167">
         <v>15</v>
       </c>
-      <c r="C34" s="186" t="s">
+      <c r="C34" s="165" t="s">
         <v>418</v>
       </c>
-      <c r="D34" s="181" t="s">
+      <c r="D34" s="160" t="s">
         <v>444</v>
       </c>
-      <c r="E34" s="182"/>
-      <c r="F34" s="188">
+      <c r="E34" s="161"/>
+      <c r="F34" s="167">
         <v>16</v>
       </c>
-      <c r="G34" s="186" t="s">
+      <c r="G34" s="165" t="s">
         <v>412</v>
       </c>
-      <c r="H34" s="181" t="s">
+      <c r="H34" s="160" t="s">
         <v>444</v>
       </c>
       <c r="I34" s="117"/>
     </row>
     <row r="35" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B35" s="188">
+      <c r="B35" s="167">
         <v>17</v>
       </c>
-      <c r="C35" s="186" t="s">
+      <c r="C35" s="165" t="s">
         <v>427</v>
       </c>
-      <c r="D35" s="181" t="s">
+      <c r="D35" s="160" t="s">
         <v>444</v>
       </c>
-      <c r="E35" s="182"/>
-      <c r="F35" s="188">
+      <c r="E35" s="161"/>
+      <c r="F35" s="167">
         <v>18</v>
       </c>
-      <c r="G35" s="186" t="s">
+      <c r="G35" s="165" t="s">
         <v>428</v>
       </c>
-      <c r="H35" s="181" t="s">
+      <c r="H35" s="160" t="s">
         <v>444</v>
       </c>
       <c r="I35" s="117"/>
     </row>
     <row r="36" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B36" s="188">
+      <c r="B36" s="167">
         <v>19</v>
       </c>
-      <c r="C36" s="186" t="s">
+      <c r="C36" s="165" t="s">
         <v>430</v>
       </c>
-      <c r="D36" s="181" t="s">
+      <c r="D36" s="160" t="s">
         <v>444</v>
       </c>
-      <c r="E36" s="182"/>
-      <c r="F36" s="188">
+      <c r="E36" s="161"/>
+      <c r="F36" s="167">
         <v>20</v>
       </c>
-      <c r="G36" s="186" t="s">
+      <c r="G36" s="165" t="s">
         <v>435</v>
       </c>
-      <c r="H36" s="181" t="s">
+      <c r="H36" s="160" t="s">
         <v>444</v>
       </c>
       <c r="I36" s="117"/>
     </row>
     <row r="37" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B37" s="188">
+      <c r="B37" s="167">
         <v>21</v>
       </c>
-      <c r="C37" s="186" t="s">
+      <c r="C37" s="165" t="s">
         <v>431</v>
       </c>
-      <c r="D37" s="181" t="s">
+      <c r="D37" s="160" t="s">
         <v>444</v>
       </c>
-      <c r="E37" s="182"/>
-      <c r="F37" s="188">
+      <c r="E37" s="161"/>
+      <c r="F37" s="167">
         <v>22</v>
       </c>
-      <c r="G37" s="186" t="s">
+      <c r="G37" s="165" t="s">
         <v>457</v>
       </c>
-      <c r="H37" s="186" t="s">
+      <c r="H37" s="165" t="s">
         <v>462</v>
       </c>
-      <c r="I37" s="185" t="s">
+      <c r="I37" s="164" t="s">
         <v>451</v>
       </c>
     </row>
     <row r="38" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B38" s="188">
+      <c r="B38" s="167">
         <v>23</v>
       </c>
-      <c r="C38" s="186" t="s">
+      <c r="C38" s="165" t="s">
         <v>432</v>
       </c>
-      <c r="D38" s="181" t="s">
+      <c r="D38" s="160" t="s">
         <v>444</v>
       </c>
-      <c r="E38" s="182"/>
-      <c r="F38" s="188">
+      <c r="E38" s="161"/>
+      <c r="F38" s="167">
         <v>24</v>
       </c>
-      <c r="G38" s="186" t="s">
+      <c r="G38" s="165" t="s">
         <v>458</v>
       </c>
-      <c r="H38" s="186" t="s">
+      <c r="H38" s="165" t="s">
         <v>463</v>
       </c>
-      <c r="I38" s="185" t="s">
+      <c r="I38" s="164" t="s">
         <v>452</v>
       </c>
     </row>
     <row r="39" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B39" s="188">
+      <c r="B39" s="167">
         <v>25</v>
       </c>
-      <c r="C39" s="186" t="s">
+      <c r="C39" s="165" t="s">
         <v>430</v>
       </c>
-      <c r="D39" s="181" t="s">
+      <c r="D39" s="160" t="s">
         <v>444</v>
       </c>
-      <c r="E39" s="182"/>
-      <c r="F39" s="188">
+      <c r="E39" s="161"/>
+      <c r="F39" s="167">
         <v>26</v>
       </c>
-      <c r="G39" s="186" t="s">
+      <c r="G39" s="165" t="s">
         <v>431</v>
       </c>
-      <c r="H39" s="181" t="s">
+      <c r="H39" s="160" t="s">
         <v>444</v>
       </c>
       <c r="I39" s="117"/>
     </row>
     <row r="40" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B40" s="188">
+      <c r="B40" s="167">
         <v>27</v>
       </c>
-      <c r="C40" s="186" t="s">
+      <c r="C40" s="165" t="s">
         <v>433</v>
       </c>
-      <c r="D40" s="181" t="s">
+      <c r="D40" s="160" t="s">
         <v>444</v>
       </c>
-      <c r="E40" s="182"/>
-      <c r="F40" s="188">
+      <c r="E40" s="161"/>
+      <c r="F40" s="167">
         <v>28</v>
       </c>
-      <c r="G40" s="186" t="s">
+      <c r="G40" s="165" t="s">
         <v>439</v>
       </c>
-      <c r="H40" s="181" t="s">
+      <c r="H40" s="160" t="s">
         <v>444</v>
       </c>
       <c r="I40" s="117"/>
     </row>
     <row r="41" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B41" s="188">
+      <c r="B41" s="167">
         <v>29</v>
       </c>
-      <c r="C41" s="186" t="s">
+      <c r="C41" s="165" t="s">
         <v>434</v>
       </c>
-      <c r="D41" s="181" t="s">
+      <c r="D41" s="160" t="s">
         <v>444</v>
       </c>
-      <c r="E41" s="182"/>
-      <c r="F41" s="188">
+      <c r="E41" s="161"/>
+      <c r="F41" s="167">
         <v>30</v>
       </c>
-      <c r="G41" s="186" t="s">
+      <c r="G41" s="165" t="s">
         <v>440</v>
       </c>
-      <c r="H41" s="186" t="s">
+      <c r="H41" s="165" t="s">
         <v>440</v>
       </c>
       <c r="I41" s="117"/>
     </row>
     <row r="42" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B42" s="188">
+      <c r="B42" s="167">
         <v>31</v>
       </c>
-      <c r="C42" s="186" t="s">
+      <c r="C42" s="165" t="s">
         <v>435</v>
       </c>
-      <c r="D42" s="181" t="s">
+      <c r="D42" s="160" t="s">
         <v>444</v>
       </c>
-      <c r="E42" s="182"/>
-      <c r="F42" s="188">
+      <c r="E42" s="161"/>
+      <c r="F42" s="167">
         <v>32</v>
       </c>
-      <c r="G42" s="186" t="s">
+      <c r="G42" s="165" t="s">
         <v>419</v>
       </c>
-      <c r="H42" s="186" t="s">
+      <c r="H42" s="165" t="s">
         <v>419</v>
       </c>
       <c r="I42" s="117"/>
     </row>
     <row r="43" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B43" s="188">
+      <c r="B43" s="167">
         <v>33</v>
       </c>
-      <c r="C43" s="186" t="s">
+      <c r="C43" s="165" t="s">
         <v>407</v>
       </c>
-      <c r="D43" s="181" t="s">
+      <c r="D43" s="160" t="s">
         <v>444</v>
       </c>
-      <c r="E43" s="182"/>
-      <c r="F43" s="188">
+      <c r="E43" s="161"/>
+      <c r="F43" s="167">
         <v>34</v>
       </c>
-      <c r="G43" s="186" t="s">
+      <c r="G43" s="165" t="s">
         <v>414</v>
       </c>
-      <c r="H43" s="186" t="s">
+      <c r="H43" s="165" t="s">
         <v>414</v>
       </c>
-      <c r="I43" s="185" t="s">
+      <c r="I43" s="164" t="s">
         <v>453</v>
       </c>
     </row>
     <row r="44" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B44" s="188">
+      <c r="B44" s="167">
         <v>35</v>
       </c>
-      <c r="C44" s="186" t="s">
+      <c r="C44" s="165" t="s">
         <v>413</v>
       </c>
-      <c r="D44" s="181" t="s">
+      <c r="D44" s="160" t="s">
         <v>444</v>
       </c>
-      <c r="E44" s="182"/>
-      <c r="F44" s="188">
+      <c r="E44" s="161"/>
+      <c r="F44" s="167">
         <v>36</v>
       </c>
-      <c r="G44" s="186" t="s">
+      <c r="G44" s="165" t="s">
         <v>420</v>
       </c>
-      <c r="H44" s="181" t="s">
+      <c r="H44" s="160" t="s">
         <v>444</v>
       </c>
       <c r="I44" s="117"/>
     </row>
     <row r="45" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B45" s="188">
+      <c r="B45" s="167">
         <v>37</v>
       </c>
-      <c r="C45" s="186" t="s">
+      <c r="C45" s="165" t="s">
         <v>436</v>
       </c>
-      <c r="D45" s="181" t="s">
+      <c r="D45" s="160" t="s">
         <v>444</v>
       </c>
-      <c r="E45" s="182"/>
-      <c r="F45" s="188">
+      <c r="E45" s="161"/>
+      <c r="F45" s="167">
         <v>38</v>
       </c>
-      <c r="G45" s="186" t="s">
+      <c r="G45" s="165" t="s">
         <v>423</v>
       </c>
-      <c r="H45" s="181" t="s">
+      <c r="H45" s="160" t="s">
         <v>444</v>
       </c>
       <c r="I45" s="117"/>
     </row>
     <row r="46" spans="2:9" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B46" s="189">
+      <c r="B46" s="168">
         <v>39</v>
       </c>
-      <c r="C46" s="187" t="s">
+      <c r="C46" s="166" t="s">
         <v>437</v>
       </c>
-      <c r="D46" s="183" t="s">
+      <c r="D46" s="162" t="s">
         <v>444</v>
       </c>
-      <c r="E46" s="184"/>
-      <c r="F46" s="189">
+      <c r="E46" s="163"/>
+      <c r="F46" s="168">
         <v>40</v>
       </c>
-      <c r="G46" s="187" t="s">
+      <c r="G46" s="166" t="s">
         <v>441</v>
       </c>
-      <c r="H46" s="183" t="s">
+      <c r="H46" s="162" t="s">
         <v>444</v>
       </c>
       <c r="I46" s="119"/>
@@ -9244,5 +9259,6 @@
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
DOC - Review Data file folder 이동
</commit_message>
<xml_diff>
--- a/MCU PCB/Plasma_LF_MCU_PinMap_20180117.xlsx
+++ b/MCU PCB/Plasma_LF_MCU_PinMap_20180117.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1319" uniqueCount="467">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1311" uniqueCount="478">
   <si>
     <t>Function</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -1862,6 +1862,50 @@
   </si>
   <si>
     <t>-</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>32.768KHz</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>8.0MHz</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>PWR_LED</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Plasma On</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>GPIO_EXTI4_Rising&amp;Falling</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>GPIO_EXTI5_Rising&amp;Falling</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>GPIO_EXTI6_Rising&amp;Falling</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>G15</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>G17</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Main PCB OP-AMP Output</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>+5V input</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1872,7 +1916,7 @@
   <numFmts count="1">
     <numFmt numFmtId="176" formatCode="0.0"/>
   </numFmts>
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1934,23 +1978,8 @@
       <charset val="129"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <sz val="11"/>
-      <name val="맑은 고딕"/>
-      <family val="3"/>
-      <charset val="129"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="맑은 고딕"/>
-      <family val="3"/>
-      <charset val="129"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
-  <fills count="15">
+  <fills count="14">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -2025,18 +2054,12 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="0" tint="-0.34998626667073579"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="4" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="13">
+  <borders count="16">
     <border>
       <left/>
       <right/>
@@ -2218,12 +2241,49 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="193">
+  <cellXfs count="189">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -2628,87 +2688,87 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="5" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="11" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="11" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="13" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="13" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="13" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="13" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="13" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="13" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="13" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="13" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="13" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="13" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="11" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -2721,9 +2781,6 @@
     <xf numFmtId="0" fontId="0" fillId="11" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -2739,40 +2796,31 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="13" borderId="5" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="13" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="13" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="14" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="14" borderId="5" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="14" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="6" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -3082,14 +3130,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:AB95"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="U74" sqref="U74"/>
+    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="W38" sqref="W38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="3.5" style="1" customWidth="1"/>
-    <col min="2" max="3" width="7.5" style="1" customWidth="1"/>
+    <col min="2" max="2" width="7.5" style="1" customWidth="1"/>
+    <col min="3" max="3" width="7.5" style="1" hidden="1" customWidth="1"/>
     <col min="4" max="4" width="7.5" style="5" customWidth="1"/>
     <col min="5" max="5" width="24.875" style="5" customWidth="1"/>
     <col min="6" max="6" width="18.125" style="5" customWidth="1"/>
@@ -3106,8 +3155,8 @@
     <col min="17" max="17" width="14.125" style="5" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="24.125" style="5" bestFit="1" customWidth="1"/>
     <col min="19" max="19" width="11.625" style="5" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="19.75" style="1" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="19" style="1" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="19.75" style="1" hidden="1" customWidth="1"/>
+    <col min="21" max="21" width="19" style="1" hidden="1" customWidth="1"/>
     <col min="22" max="22" width="25.25" style="5" bestFit="1" customWidth="1"/>
     <col min="23" max="23" width="14.25" style="5" bestFit="1" customWidth="1"/>
     <col min="24" max="24" width="14.125" style="5" bestFit="1" customWidth="1"/>
@@ -3142,10 +3191,10 @@
       <c r="X2" s="1"/>
     </row>
     <row r="3" spans="2:27" x14ac:dyDescent="0.3">
-      <c r="B3" s="184" t="s">
+      <c r="B3" s="159" t="s">
         <v>3</v>
       </c>
-      <c r="C3" s="185"/>
+      <c r="C3" s="160"/>
       <c r="D3" s="2">
         <v>128</v>
       </c>
@@ -3173,10 +3222,10 @@
       </c>
     </row>
     <row r="4" spans="2:27" x14ac:dyDescent="0.3">
-      <c r="B4" s="186" t="s">
+      <c r="B4" s="161" t="s">
         <v>5</v>
       </c>
-      <c r="C4" s="187"/>
+      <c r="C4" s="162"/>
       <c r="D4" s="3">
         <v>16</v>
       </c>
@@ -3206,10 +3255,10 @@
       </c>
     </row>
     <row r="5" spans="2:27" x14ac:dyDescent="0.3">
-      <c r="B5" s="186" t="s">
+      <c r="B5" s="161" t="s">
         <v>6</v>
       </c>
-      <c r="C5" s="187"/>
+      <c r="C5" s="162"/>
       <c r="D5" s="3">
         <v>48</v>
       </c>
@@ -3241,10 +3290,10 @@
       </c>
     </row>
     <row r="6" spans="2:27" x14ac:dyDescent="0.3">
-      <c r="B6" s="186" t="s">
+      <c r="B6" s="161" t="s">
         <v>9</v>
       </c>
-      <c r="C6" s="187"/>
+      <c r="C6" s="162"/>
       <c r="D6" s="3" t="s">
         <v>10</v>
       </c>
@@ -3268,10 +3317,10 @@
       <c r="X6" s="18"/>
     </row>
     <row r="7" spans="2:27" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B7" s="188" t="s">
+      <c r="B7" s="163" t="s">
         <v>12</v>
       </c>
-      <c r="C7" s="189"/>
+      <c r="C7" s="164"/>
       <c r="D7" s="4" t="s">
         <v>13</v>
       </c>
@@ -3390,51 +3439,51 @@
     </row>
     <row r="13" spans="2:27" ht="17.25" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="14" spans="2:27" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B14" s="181" t="s">
+      <c r="B14" s="165" t="s">
         <v>178</v>
       </c>
-      <c r="C14" s="175"/>
-      <c r="D14" s="175" t="s">
+      <c r="C14" s="166"/>
+      <c r="D14" s="166" t="s">
         <v>163</v>
       </c>
-      <c r="E14" s="175" t="s">
+      <c r="E14" s="166" t="s">
         <v>165</v>
       </c>
-      <c r="F14" s="176"/>
-      <c r="G14" s="169" t="s">
+      <c r="F14" s="175"/>
+      <c r="G14" s="167" t="s">
         <v>14</v>
       </c>
-      <c r="H14" s="182"/>
-      <c r="I14" s="169" t="s">
+      <c r="H14" s="168"/>
+      <c r="I14" s="167" t="s">
         <v>311</v>
       </c>
-      <c r="J14" s="182"/>
-      <c r="K14" s="169" t="s">
+      <c r="J14" s="168"/>
+      <c r="K14" s="167" t="s">
         <v>312</v>
       </c>
-      <c r="L14" s="170"/>
+      <c r="L14" s="169"/>
       <c r="M14" s="23"/>
       <c r="N14" s="38"/>
-      <c r="O14" s="169" t="s">
+      <c r="O14" s="167" t="s">
         <v>14</v>
       </c>
-      <c r="P14" s="170"/>
-      <c r="Q14" s="170" t="s">
+      <c r="P14" s="169"/>
+      <c r="Q14" s="169" t="s">
         <v>162</v>
       </c>
-      <c r="R14" s="170"/>
+      <c r="R14" s="169"/>
       <c r="S14" s="58"/>
       <c r="T14" s="36"/>
-      <c r="V14" s="169" t="s">
+      <c r="V14" s="167" t="s">
         <v>14</v>
       </c>
-      <c r="W14" s="170"/>
-      <c r="X14" s="170" t="s">
+      <c r="W14" s="169"/>
+      <c r="X14" s="185" t="s">
         <v>383</v>
       </c>
-      <c r="Y14" s="170"/>
-      <c r="Z14" s="58"/>
-      <c r="AA14" s="36"/>
+      <c r="Y14" s="186"/>
+      <c r="Z14" s="186"/>
+      <c r="AA14" s="187"/>
     </row>
     <row r="15" spans="2:27" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B15" s="7" t="s">
@@ -3443,7 +3492,7 @@
       <c r="C15" s="15" t="s">
         <v>180</v>
       </c>
-      <c r="D15" s="183"/>
+      <c r="D15" s="170"/>
       <c r="E15" s="15" t="s">
         <v>248</v>
       </c>
@@ -3495,16 +3544,16 @@
       <c r="V15" s="59" t="s">
         <v>0</v>
       </c>
-      <c r="W15" s="146" t="s">
+      <c r="W15" s="144" t="s">
         <v>16</v>
       </c>
-      <c r="X15" s="146" t="s">
+      <c r="X15" s="144" t="s">
         <v>17</v>
       </c>
-      <c r="Y15" s="146" t="s">
+      <c r="Y15" s="144" t="s">
         <v>0</v>
       </c>
-      <c r="Z15" s="146" t="s">
+      <c r="Z15" s="144" t="s">
         <v>18</v>
       </c>
       <c r="AA15" s="10" t="s">
@@ -3521,10 +3570,10 @@
       <c r="D16" s="21" t="s">
         <v>164</v>
       </c>
-      <c r="E16" s="177" t="s">
+      <c r="E16" s="176" t="s">
         <v>176</v>
       </c>
-      <c r="F16" s="178"/>
+      <c r="F16" s="177"/>
       <c r="G16" s="52"/>
       <c r="H16" s="71"/>
       <c r="I16" s="81"/>
@@ -3613,7 +3662,7 @@
       <c r="Z17" s="8" t="s">
         <v>72</v>
       </c>
-      <c r="AA17" s="18"/>
+      <c r="AA17" s="40"/>
     </row>
     <row r="18" spans="2:27" x14ac:dyDescent="0.3">
       <c r="B18" s="28">
@@ -3657,22 +3706,22 @@
         <v>72</v>
       </c>
       <c r="T18" s="18"/>
-      <c r="V18" s="190" t="s">
+      <c r="V18" s="184" t="s">
         <v>166</v>
       </c>
-      <c r="W18" s="191" t="s">
+      <c r="W18" s="180" t="s">
         <v>379</v>
       </c>
-      <c r="X18" s="191" t="s">
-        <v>72</v>
-      </c>
-      <c r="Y18" s="191" t="s">
-        <v>72</v>
-      </c>
-      <c r="Z18" s="191" t="s">
-        <v>72</v>
-      </c>
-      <c r="AA18" s="192"/>
+      <c r="X18" s="180" t="s">
+        <v>72</v>
+      </c>
+      <c r="Y18" s="180" t="s">
+        <v>467</v>
+      </c>
+      <c r="Z18" s="180" t="s">
+        <v>72</v>
+      </c>
+      <c r="AA18" s="181"/>
     </row>
     <row r="19" spans="2:27" x14ac:dyDescent="0.3">
       <c r="B19" s="28">
@@ -3716,22 +3765,22 @@
         <v>72</v>
       </c>
       <c r="T19" s="18"/>
-      <c r="V19" s="190" t="s">
+      <c r="V19" s="184" t="s">
         <v>167</v>
       </c>
-      <c r="W19" s="191" t="s">
+      <c r="W19" s="180" t="s">
         <v>379</v>
       </c>
-      <c r="X19" s="191" t="s">
-        <v>72</v>
-      </c>
-      <c r="Y19" s="191" t="s">
-        <v>72</v>
-      </c>
-      <c r="Z19" s="191" t="s">
-        <v>72</v>
-      </c>
-      <c r="AA19" s="192"/>
+      <c r="X19" s="180" t="s">
+        <v>72</v>
+      </c>
+      <c r="Y19" s="180" t="s">
+        <v>467</v>
+      </c>
+      <c r="Z19" s="180" t="s">
+        <v>72</v>
+      </c>
+      <c r="AA19" s="181"/>
     </row>
     <row r="20" spans="2:27" x14ac:dyDescent="0.3">
       <c r="B20" s="28">
@@ -3773,22 +3822,22 @@
         <v>72</v>
       </c>
       <c r="T20" s="18"/>
-      <c r="V20" s="190" t="s">
+      <c r="V20" s="184" t="s">
         <v>171</v>
       </c>
-      <c r="W20" s="191" t="s">
+      <c r="W20" s="180" t="s">
         <v>379</v>
       </c>
-      <c r="X20" s="191" t="s">
-        <v>72</v>
-      </c>
-      <c r="Y20" s="191" t="s">
-        <v>72</v>
-      </c>
-      <c r="Z20" s="191" t="s">
-        <v>72</v>
-      </c>
-      <c r="AA20" s="192"/>
+      <c r="X20" s="180" t="s">
+        <v>72</v>
+      </c>
+      <c r="Y20" s="180" t="s">
+        <v>468</v>
+      </c>
+      <c r="Z20" s="180" t="s">
+        <v>72</v>
+      </c>
+      <c r="AA20" s="181"/>
     </row>
     <row r="21" spans="2:27" x14ac:dyDescent="0.3">
       <c r="B21" s="28">
@@ -3830,22 +3879,22 @@
         <v>72</v>
       </c>
       <c r="T21" s="18"/>
-      <c r="V21" s="190" t="s">
+      <c r="V21" s="184" t="s">
         <v>175</v>
       </c>
-      <c r="W21" s="191" t="s">
+      <c r="W21" s="180" t="s">
         <v>379</v>
       </c>
-      <c r="X21" s="191" t="s">
-        <v>72</v>
-      </c>
-      <c r="Y21" s="191" t="s">
-        <v>72</v>
-      </c>
-      <c r="Z21" s="191" t="s">
-        <v>72</v>
-      </c>
-      <c r="AA21" s="192"/>
+      <c r="X21" s="180" t="s">
+        <v>72</v>
+      </c>
+      <c r="Y21" s="180" t="s">
+        <v>468</v>
+      </c>
+      <c r="Z21" s="180" t="s">
+        <v>72</v>
+      </c>
+      <c r="AA21" s="181"/>
     </row>
     <row r="22" spans="2:27" x14ac:dyDescent="0.3">
       <c r="B22" s="28">
@@ -3857,10 +3906,10 @@
       <c r="D22" s="13" t="s">
         <v>170</v>
       </c>
-      <c r="E22" s="179" t="s">
+      <c r="E22" s="178" t="s">
         <v>177</v>
       </c>
-      <c r="F22" s="180"/>
+      <c r="F22" s="179"/>
       <c r="G22" s="66"/>
       <c r="H22" s="40"/>
       <c r="I22" s="29"/>
@@ -3900,7 +3949,7 @@
       <c r="Z22" s="25" t="s">
         <v>41</v>
       </c>
-      <c r="AA22" s="18"/>
+      <c r="AA22" s="83"/>
     </row>
     <row r="23" spans="2:27" x14ac:dyDescent="0.3">
       <c r="B23" s="28">
@@ -3971,7 +4020,7 @@
       <c r="Z23" s="8" t="s">
         <v>72</v>
       </c>
-      <c r="AA23" s="18"/>
+      <c r="AA23" s="40"/>
     </row>
     <row r="24" spans="2:27" x14ac:dyDescent="0.3">
       <c r="B24" s="28">
@@ -4034,15 +4083,15 @@
         <v>22</v>
       </c>
       <c r="X24" s="84" t="s">
-        <v>445</v>
-      </c>
-      <c r="Y24" s="84" t="s">
-        <v>465</v>
+        <v>447</v>
+      </c>
+      <c r="Y24" s="143" t="s">
+        <v>72</v>
       </c>
       <c r="Z24" s="143" t="s">
         <v>72</v>
       </c>
-      <c r="AA24" s="18"/>
+      <c r="AA24" s="83"/>
     </row>
     <row r="25" spans="2:27" x14ac:dyDescent="0.3">
       <c r="B25" s="28">
@@ -4113,7 +4162,7 @@
       <c r="Z25" s="143" t="s">
         <v>72</v>
       </c>
-      <c r="AA25" s="18"/>
+      <c r="AA25" s="83"/>
     </row>
     <row r="26" spans="2:27" x14ac:dyDescent="0.3">
       <c r="B26" s="28">
@@ -4164,15 +4213,15 @@
         <v>22</v>
       </c>
       <c r="X26" s="84" t="s">
-        <v>447</v>
-      </c>
-      <c r="Y26" s="143" t="s">
-        <v>466</v>
+        <v>445</v>
+      </c>
+      <c r="Y26" s="84" t="s">
+        <v>465</v>
       </c>
       <c r="Z26" s="143" t="s">
         <v>72</v>
       </c>
-      <c r="AA26" s="18"/>
+      <c r="AA26" s="83"/>
     </row>
     <row r="27" spans="2:27" x14ac:dyDescent="0.3">
       <c r="B27" s="30">
@@ -4203,10 +4252,10 @@
       <c r="S27" s="55"/>
       <c r="T27" s="42"/>
       <c r="V27" s="30"/>
-      <c r="W27" s="144"/>
-      <c r="X27" s="144"/>
-      <c r="Y27" s="144"/>
-      <c r="Z27" s="144"/>
+      <c r="W27" s="157"/>
+      <c r="X27" s="157"/>
+      <c r="Y27" s="157"/>
+      <c r="Z27" s="157"/>
       <c r="AA27" s="42"/>
     </row>
     <row r="28" spans="2:27" x14ac:dyDescent="0.3">
@@ -4238,10 +4287,10 @@
       <c r="S28" s="55"/>
       <c r="T28" s="42"/>
       <c r="V28" s="30"/>
-      <c r="W28" s="144"/>
-      <c r="X28" s="144"/>
-      <c r="Y28" s="144"/>
-      <c r="Z28" s="144"/>
+      <c r="W28" s="157"/>
+      <c r="X28" s="157"/>
+      <c r="Y28" s="157"/>
+      <c r="Z28" s="157"/>
       <c r="AA28" s="42"/>
     </row>
     <row r="29" spans="2:27" x14ac:dyDescent="0.3">
@@ -4301,7 +4350,7 @@
       <c r="Z29" s="8" t="s">
         <v>72</v>
       </c>
-      <c r="AA29" s="18"/>
+      <c r="AA29" s="40"/>
     </row>
     <row r="30" spans="2:27" ht="33" x14ac:dyDescent="0.3">
       <c r="B30" s="28">
@@ -4360,7 +4409,7 @@
       <c r="Z30" s="8" t="s">
         <v>72</v>
       </c>
-      <c r="AA30" s="18"/>
+      <c r="AA30" s="40"/>
     </row>
     <row r="31" spans="2:27" x14ac:dyDescent="0.3">
       <c r="B31" s="28">
@@ -4419,7 +4468,7 @@
       <c r="Z31" s="8" t="s">
         <v>72</v>
       </c>
-      <c r="AA31" s="18"/>
+      <c r="AA31" s="40"/>
     </row>
     <row r="32" spans="2:27" x14ac:dyDescent="0.3">
       <c r="B32" s="28">
@@ -4478,7 +4527,7 @@
       <c r="Z32" s="8" t="s">
         <v>72</v>
       </c>
-      <c r="AA32" s="18"/>
+      <c r="AA32" s="40"/>
     </row>
     <row r="33" spans="2:28" x14ac:dyDescent="0.3">
       <c r="B33" s="30">
@@ -4509,10 +4558,10 @@
       <c r="S33" s="55"/>
       <c r="T33" s="42"/>
       <c r="V33" s="30"/>
-      <c r="W33" s="144"/>
-      <c r="X33" s="144"/>
-      <c r="Y33" s="144"/>
-      <c r="Z33" s="144"/>
+      <c r="W33" s="157"/>
+      <c r="X33" s="157"/>
+      <c r="Y33" s="157"/>
+      <c r="Z33" s="157"/>
       <c r="AA33" s="42"/>
     </row>
     <row r="34" spans="2:28" x14ac:dyDescent="0.3">
@@ -4544,10 +4593,10 @@
       <c r="S34" s="55"/>
       <c r="T34" s="42"/>
       <c r="V34" s="30"/>
-      <c r="W34" s="144"/>
-      <c r="X34" s="144"/>
-      <c r="Y34" s="144"/>
-      <c r="Z34" s="144"/>
+      <c r="W34" s="157"/>
+      <c r="X34" s="157"/>
+      <c r="Y34" s="157"/>
+      <c r="Z34" s="157"/>
       <c r="AA34" s="42"/>
     </row>
     <row r="35" spans="2:28" ht="33" x14ac:dyDescent="0.3">
@@ -4604,22 +4653,22 @@
         <v>72</v>
       </c>
       <c r="T35" s="18"/>
-      <c r="V35" s="29" t="s">
-        <v>378</v>
-      </c>
-      <c r="W35" s="8" t="s">
+      <c r="V35" s="182" t="s">
+        <v>471</v>
+      </c>
+      <c r="W35" s="143" t="s">
         <v>379</v>
       </c>
-      <c r="X35" s="8" t="s">
-        <v>72</v>
-      </c>
-      <c r="Y35" s="8" t="s">
-        <v>72</v>
-      </c>
-      <c r="Z35" s="8" t="s">
-        <v>72</v>
-      </c>
-      <c r="AA35" s="18"/>
+      <c r="X35" s="143" t="s">
+        <v>440</v>
+      </c>
+      <c r="Y35" s="143" t="s">
+        <v>72</v>
+      </c>
+      <c r="Z35" s="143" t="s">
+        <v>72</v>
+      </c>
+      <c r="AA35" s="136"/>
     </row>
     <row r="36" spans="2:28" x14ac:dyDescent="0.3">
       <c r="B36" s="28">
@@ -4675,22 +4724,22 @@
         <v>72</v>
       </c>
       <c r="T36" s="18"/>
-      <c r="V36" s="29" t="s">
-        <v>378</v>
-      </c>
-      <c r="W36" s="8" t="s">
+      <c r="V36" s="182" t="s">
+        <v>472</v>
+      </c>
+      <c r="W36" s="143" t="s">
         <v>379</v>
       </c>
-      <c r="X36" s="8" t="s">
-        <v>72</v>
-      </c>
-      <c r="Y36" s="8" t="s">
-        <v>72</v>
-      </c>
-      <c r="Z36" s="8" t="s">
-        <v>72</v>
-      </c>
-      <c r="AA36" s="18"/>
+      <c r="X36" s="143" t="s">
+        <v>474</v>
+      </c>
+      <c r="Y36" s="143" t="s">
+        <v>72</v>
+      </c>
+      <c r="Z36" s="143" t="s">
+        <v>72</v>
+      </c>
+      <c r="AA36" s="136"/>
     </row>
     <row r="37" spans="2:28" ht="49.5" x14ac:dyDescent="0.3">
       <c r="B37" s="28">
@@ -4748,22 +4797,24 @@
         <v>25</v>
       </c>
       <c r="T37" s="141"/>
-      <c r="V37" s="149" t="s">
-        <v>102</v>
-      </c>
-      <c r="W37" s="148" t="s">
-        <v>22</v>
-      </c>
-      <c r="X37" s="148" t="s">
-        <v>103</v>
-      </c>
-      <c r="Y37" s="148" t="s">
-        <v>104</v>
-      </c>
-      <c r="Z37" s="148" t="s">
-        <v>25</v>
-      </c>
-      <c r="AA37" s="141"/>
+      <c r="V37" s="183" t="s">
+        <v>473</v>
+      </c>
+      <c r="W37" s="143" t="s">
+        <v>379</v>
+      </c>
+      <c r="X37" s="143" t="s">
+        <v>475</v>
+      </c>
+      <c r="Y37" s="143" t="s">
+        <v>476</v>
+      </c>
+      <c r="Z37" s="143" t="s">
+        <v>72</v>
+      </c>
+      <c r="AA37" s="188" t="s">
+        <v>477</v>
+      </c>
     </row>
     <row r="38" spans="2:28" ht="49.5" x14ac:dyDescent="0.3">
       <c r="B38" s="28">
@@ -4832,7 +4883,7 @@
       <c r="Z38" s="8" t="s">
         <v>72</v>
       </c>
-      <c r="AA38" s="18"/>
+      <c r="AA38" s="40"/>
     </row>
     <row r="39" spans="2:28" x14ac:dyDescent="0.3">
       <c r="B39" s="28">
@@ -4901,7 +4952,7 @@
       <c r="Z39" s="8" t="s">
         <v>72</v>
       </c>
-      <c r="AA39" s="18"/>
+      <c r="AA39" s="40"/>
     </row>
     <row r="40" spans="2:28" x14ac:dyDescent="0.3">
       <c r="B40" s="28">
@@ -4960,25 +5011,22 @@
       <c r="U40" s="1" t="s">
         <v>310</v>
       </c>
-      <c r="V40" s="150" t="s">
-        <v>318</v>
-      </c>
-      <c r="W40" s="151" t="s">
-        <v>293</v>
-      </c>
-      <c r="X40" s="151" t="s">
-        <v>267</v>
-      </c>
-      <c r="Y40" s="151" t="s">
-        <v>259</v>
-      </c>
-      <c r="Z40" s="151" t="s">
-        <v>25</v>
-      </c>
-      <c r="AA40" s="152"/>
-      <c r="AB40" s="1" t="s">
-        <v>310</v>
-      </c>
+      <c r="V40" s="29" t="s">
+        <v>378</v>
+      </c>
+      <c r="W40" s="8" t="s">
+        <v>379</v>
+      </c>
+      <c r="X40" s="8" t="s">
+        <v>72</v>
+      </c>
+      <c r="Y40" s="8" t="s">
+        <v>72</v>
+      </c>
+      <c r="Z40" s="8" t="s">
+        <v>72</v>
+      </c>
+      <c r="AA40" s="40"/>
     </row>
     <row r="41" spans="2:28" ht="33" x14ac:dyDescent="0.3">
       <c r="B41" s="28">
@@ -5034,22 +5082,22 @@
         <v>25</v>
       </c>
       <c r="T41" s="83"/>
-      <c r="V41" s="149" t="s">
-        <v>21</v>
-      </c>
-      <c r="W41" s="148" t="s">
-        <v>22</v>
-      </c>
-      <c r="X41" s="148" t="s">
-        <v>258</v>
-      </c>
-      <c r="Y41" s="148" t="s">
-        <v>268</v>
-      </c>
-      <c r="Z41" s="148" t="s">
-        <v>25</v>
-      </c>
-      <c r="AA41" s="152"/>
+      <c r="V41" s="29" t="s">
+        <v>378</v>
+      </c>
+      <c r="W41" s="8" t="s">
+        <v>379</v>
+      </c>
+      <c r="X41" s="8" t="s">
+        <v>72</v>
+      </c>
+      <c r="Y41" s="8" t="s">
+        <v>72</v>
+      </c>
+      <c r="Z41" s="8" t="s">
+        <v>72</v>
+      </c>
+      <c r="AA41" s="40"/>
     </row>
     <row r="42" spans="2:28" ht="33" x14ac:dyDescent="0.3">
       <c r="B42" s="28">
@@ -5108,25 +5156,23 @@
       <c r="U42" s="134" t="s">
         <v>380</v>
       </c>
-      <c r="V42" s="153" t="s">
-        <v>313</v>
-      </c>
-      <c r="W42" s="154" t="s">
-        <v>22</v>
-      </c>
-      <c r="X42" s="154" t="s">
-        <v>315</v>
-      </c>
-      <c r="Y42" s="154" t="s">
-        <v>290</v>
-      </c>
-      <c r="Z42" s="154"/>
-      <c r="AA42" s="155" t="s">
-        <v>275</v>
-      </c>
-      <c r="AB42" s="134" t="s">
-        <v>380</v>
-      </c>
+      <c r="V42" s="29" t="s">
+        <v>378</v>
+      </c>
+      <c r="W42" s="8" t="s">
+        <v>379</v>
+      </c>
+      <c r="X42" s="8" t="s">
+        <v>72</v>
+      </c>
+      <c r="Y42" s="8" t="s">
+        <v>72</v>
+      </c>
+      <c r="Z42" s="8" t="s">
+        <v>72</v>
+      </c>
+      <c r="AA42" s="40"/>
+      <c r="AB42" s="134"/>
     </row>
     <row r="43" spans="2:28" x14ac:dyDescent="0.3">
       <c r="B43" s="28">
@@ -5197,7 +5243,7 @@
       <c r="Z43" s="8" t="s">
         <v>72</v>
       </c>
-      <c r="AA43" s="18"/>
+      <c r="AA43" s="40"/>
     </row>
     <row r="44" spans="2:28" x14ac:dyDescent="0.3">
       <c r="B44" s="28">
@@ -5268,7 +5314,7 @@
       <c r="Z44" s="8" t="s">
         <v>72</v>
       </c>
-      <c r="AA44" s="18"/>
+      <c r="AA44" s="40"/>
     </row>
     <row r="45" spans="2:28" ht="33" x14ac:dyDescent="0.3">
       <c r="B45" s="28">
@@ -5337,7 +5383,7 @@
       <c r="Z45" s="8" t="s">
         <v>72</v>
       </c>
-      <c r="AA45" s="18"/>
+      <c r="AA45" s="40"/>
     </row>
     <row r="46" spans="2:28" x14ac:dyDescent="0.3">
       <c r="B46" s="30">
@@ -5368,10 +5414,10 @@
       <c r="S46" s="55"/>
       <c r="T46" s="42"/>
       <c r="V46" s="30"/>
-      <c r="W46" s="144"/>
-      <c r="X46" s="144"/>
-      <c r="Y46" s="144"/>
-      <c r="Z46" s="144"/>
+      <c r="W46" s="157"/>
+      <c r="X46" s="157"/>
+      <c r="Y46" s="157"/>
+      <c r="Z46" s="157"/>
       <c r="AA46" s="42"/>
     </row>
     <row r="47" spans="2:28" x14ac:dyDescent="0.3">
@@ -5403,10 +5449,10 @@
       <c r="S47" s="55"/>
       <c r="T47" s="42"/>
       <c r="V47" s="30"/>
-      <c r="W47" s="144"/>
-      <c r="X47" s="144"/>
-      <c r="Y47" s="144"/>
-      <c r="Z47" s="144"/>
+      <c r="W47" s="157"/>
+      <c r="X47" s="157"/>
+      <c r="Y47" s="157"/>
+      <c r="Z47" s="157"/>
       <c r="AA47" s="42"/>
     </row>
     <row r="48" spans="2:28" ht="49.5" x14ac:dyDescent="0.3">
@@ -5454,27 +5500,24 @@
       <c r="U48" s="1" t="s">
         <v>308</v>
       </c>
-      <c r="V48" s="149" t="s">
-        <v>21</v>
-      </c>
-      <c r="W48" s="148" t="s">
-        <v>293</v>
-      </c>
-      <c r="X48" s="148" t="s">
-        <v>294</v>
-      </c>
-      <c r="Y48" s="148" t="s">
-        <v>290</v>
-      </c>
-      <c r="Z48" s="148" t="s">
-        <v>25</v>
-      </c>
-      <c r="AA48" s="152"/>
-      <c r="AB48" s="1" t="s">
-        <v>308</v>
-      </c>
-    </row>
-    <row r="49" spans="2:28" ht="33" x14ac:dyDescent="0.3">
+      <c r="V48" s="29" t="s">
+        <v>378</v>
+      </c>
+      <c r="W48" s="8" t="s">
+        <v>379</v>
+      </c>
+      <c r="X48" s="8" t="s">
+        <v>72</v>
+      </c>
+      <c r="Y48" s="8" t="s">
+        <v>72</v>
+      </c>
+      <c r="Z48" s="8" t="s">
+        <v>72</v>
+      </c>
+      <c r="AA48" s="40"/>
+    </row>
+    <row r="49" spans="2:27" ht="33" x14ac:dyDescent="0.3">
       <c r="B49" s="28">
         <v>34</v>
       </c>
@@ -5531,9 +5574,9 @@
       <c r="Z49" s="8" t="s">
         <v>72</v>
       </c>
-      <c r="AA49" s="18"/>
-    </row>
-    <row r="50" spans="2:28" ht="49.5" x14ac:dyDescent="0.3">
+      <c r="AA49" s="40"/>
+    </row>
+    <row r="50" spans="2:27" ht="49.5" x14ac:dyDescent="0.3">
       <c r="B50" s="28">
         <v>35</v>
       </c>
@@ -5590,9 +5633,9 @@
       <c r="Z50" s="8" t="s">
         <v>72</v>
       </c>
-      <c r="AA50" s="18"/>
-    </row>
-    <row r="51" spans="2:28" ht="33" x14ac:dyDescent="0.3">
+      <c r="AA50" s="40"/>
+    </row>
+    <row r="51" spans="2:27" ht="33" x14ac:dyDescent="0.3">
       <c r="B51" s="28">
         <v>36</v>
       </c>
@@ -5651,29 +5694,24 @@
       <c r="U51" s="1" t="s">
         <v>309</v>
       </c>
-      <c r="V51" s="147" t="s">
-        <v>275</v>
-      </c>
-      <c r="W51" s="148" t="s">
-        <v>22</v>
-      </c>
-      <c r="X51" s="148" t="s">
-        <v>289</v>
-      </c>
-      <c r="Y51" s="148" t="s">
-        <v>272</v>
-      </c>
-      <c r="Z51" s="148" t="s">
-        <v>25</v>
-      </c>
-      <c r="AA51" s="152" t="s">
-        <v>304</v>
-      </c>
-      <c r="AB51" s="1" t="s">
-        <v>309</v>
-      </c>
-    </row>
-    <row r="52" spans="2:28" x14ac:dyDescent="0.3">
+      <c r="V51" s="29" t="s">
+        <v>378</v>
+      </c>
+      <c r="W51" s="8" t="s">
+        <v>379</v>
+      </c>
+      <c r="X51" s="8" t="s">
+        <v>72</v>
+      </c>
+      <c r="Y51" s="8" t="s">
+        <v>72</v>
+      </c>
+      <c r="Z51" s="8" t="s">
+        <v>72</v>
+      </c>
+      <c r="AA51" s="40"/>
+    </row>
+    <row r="52" spans="2:27" x14ac:dyDescent="0.3">
       <c r="B52" s="28">
         <v>37</v>
       </c>
@@ -5742,9 +5780,9 @@
       <c r="Z52" s="8" t="s">
         <v>72</v>
       </c>
-      <c r="AA52" s="18"/>
-    </row>
-    <row r="53" spans="2:28" x14ac:dyDescent="0.3">
+      <c r="AA52" s="40"/>
+    </row>
+    <row r="53" spans="2:27" x14ac:dyDescent="0.3">
       <c r="B53" s="28">
         <v>38</v>
       </c>
@@ -5803,29 +5841,24 @@
       <c r="U53" s="1" t="s">
         <v>310</v>
       </c>
-      <c r="V53" s="150" t="s">
-        <v>319</v>
-      </c>
-      <c r="W53" s="151" t="s">
-        <v>22</v>
-      </c>
-      <c r="X53" s="151" t="s">
-        <v>316</v>
-      </c>
-      <c r="Y53" s="151" t="s">
-        <v>272</v>
-      </c>
-      <c r="Z53" s="151" t="s">
-        <v>25</v>
-      </c>
-      <c r="AA53" s="156" t="s">
-        <v>275</v>
-      </c>
-      <c r="AB53" s="1" t="s">
-        <v>310</v>
-      </c>
-    </row>
-    <row r="54" spans="2:28" x14ac:dyDescent="0.3">
+      <c r="V53" s="29" t="s">
+        <v>378</v>
+      </c>
+      <c r="W53" s="8" t="s">
+        <v>379</v>
+      </c>
+      <c r="X53" s="8" t="s">
+        <v>72</v>
+      </c>
+      <c r="Y53" s="8" t="s">
+        <v>72</v>
+      </c>
+      <c r="Z53" s="8" t="s">
+        <v>72</v>
+      </c>
+      <c r="AA53" s="40"/>
+    </row>
+    <row r="54" spans="2:27" x14ac:dyDescent="0.3">
       <c r="B54" s="28">
         <v>39</v>
       </c>
@@ -5894,9 +5927,9 @@
       <c r="Z54" s="8" t="s">
         <v>72</v>
       </c>
-      <c r="AA54" s="18"/>
-    </row>
-    <row r="55" spans="2:28" x14ac:dyDescent="0.3">
+      <c r="AA54" s="40"/>
+    </row>
+    <row r="55" spans="2:27" x14ac:dyDescent="0.3">
       <c r="B55" s="28">
         <v>40</v>
       </c>
@@ -5965,9 +5998,9 @@
       <c r="Z55" s="8" t="s">
         <v>72</v>
       </c>
-      <c r="AA55" s="18"/>
-    </row>
-    <row r="56" spans="2:28" ht="33" x14ac:dyDescent="0.3">
+      <c r="AA55" s="40"/>
+    </row>
+    <row r="56" spans="2:27" ht="33" x14ac:dyDescent="0.3">
       <c r="B56" s="28">
         <v>41</v>
       </c>
@@ -6026,7 +6059,7 @@
       </c>
       <c r="AA56" s="141"/>
     </row>
-    <row r="57" spans="2:28" ht="33" x14ac:dyDescent="0.3">
+    <row r="57" spans="2:27" ht="33" x14ac:dyDescent="0.3">
       <c r="B57" s="28">
         <v>42</v>
       </c>
@@ -6091,7 +6124,7 @@
       </c>
       <c r="AA57" s="96"/>
     </row>
-    <row r="58" spans="2:28" ht="33" x14ac:dyDescent="0.3">
+    <row r="58" spans="2:27" ht="33" x14ac:dyDescent="0.3">
       <c r="B58" s="28">
         <v>43</v>
       </c>
@@ -6158,7 +6191,7 @@
       </c>
       <c r="AA58" s="96"/>
     </row>
-    <row r="59" spans="2:28" ht="33" x14ac:dyDescent="0.3">
+    <row r="59" spans="2:27" ht="33" x14ac:dyDescent="0.3">
       <c r="B59" s="28">
         <v>44</v>
       </c>
@@ -6225,7 +6258,7 @@
       </c>
       <c r="AA59" s="141"/>
     </row>
-    <row r="60" spans="2:28" ht="33" x14ac:dyDescent="0.3">
+    <row r="60" spans="2:27" ht="33" x14ac:dyDescent="0.3">
       <c r="B60" s="28">
         <v>45</v>
       </c>
@@ -6277,24 +6310,24 @@
         <v>25</v>
       </c>
       <c r="T60" s="136"/>
-      <c r="V60" s="149" t="s">
-        <v>21</v>
-      </c>
-      <c r="W60" s="148" t="s">
-        <v>293</v>
-      </c>
-      <c r="X60" s="148" t="s">
-        <v>279</v>
-      </c>
-      <c r="Y60" s="148" t="s">
-        <v>250</v>
-      </c>
-      <c r="Z60" s="148" t="s">
-        <v>25</v>
-      </c>
-      <c r="AA60" s="152"/>
-    </row>
-    <row r="61" spans="2:28" x14ac:dyDescent="0.3">
+      <c r="V60" s="29" t="s">
+        <v>378</v>
+      </c>
+      <c r="W60" s="8" t="s">
+        <v>379</v>
+      </c>
+      <c r="X60" s="8" t="s">
+        <v>72</v>
+      </c>
+      <c r="Y60" s="8" t="s">
+        <v>72</v>
+      </c>
+      <c r="Z60" s="8" t="s">
+        <v>72</v>
+      </c>
+      <c r="AA60" s="40"/>
+    </row>
+    <row r="61" spans="2:27" x14ac:dyDescent="0.3">
       <c r="B61" s="28">
         <v>46</v>
       </c>
@@ -6363,7 +6396,7 @@
       </c>
       <c r="AA61" s="105"/>
     </row>
-    <row r="62" spans="2:28" x14ac:dyDescent="0.3">
+    <row r="62" spans="2:27" x14ac:dyDescent="0.3">
       <c r="B62" s="30">
         <v>47</v>
       </c>
@@ -6392,13 +6425,13 @@
       <c r="S62" s="55"/>
       <c r="T62" s="42"/>
       <c r="V62" s="30"/>
-      <c r="W62" s="144"/>
-      <c r="X62" s="144"/>
-      <c r="Y62" s="144"/>
-      <c r="Z62" s="144"/>
+      <c r="W62" s="157"/>
+      <c r="X62" s="157"/>
+      <c r="Y62" s="157"/>
+      <c r="Z62" s="157"/>
       <c r="AA62" s="42"/>
     </row>
-    <row r="63" spans="2:28" x14ac:dyDescent="0.3">
+    <row r="63" spans="2:27" x14ac:dyDescent="0.3">
       <c r="B63" s="30">
         <v>48</v>
       </c>
@@ -6427,13 +6460,13 @@
       <c r="S63" s="55"/>
       <c r="T63" s="42"/>
       <c r="V63" s="30"/>
-      <c r="W63" s="144"/>
-      <c r="X63" s="144"/>
-      <c r="Y63" s="144"/>
-      <c r="Z63" s="144"/>
+      <c r="W63" s="157"/>
+      <c r="X63" s="157"/>
+      <c r="Y63" s="157"/>
+      <c r="Z63" s="157"/>
       <c r="AA63" s="42"/>
     </row>
-    <row r="64" spans="2:28" x14ac:dyDescent="0.3">
+    <row r="64" spans="2:27" x14ac:dyDescent="0.3">
       <c r="B64" s="28">
         <v>49</v>
       </c>
@@ -6502,7 +6535,7 @@
       </c>
       <c r="AA64" s="105"/>
     </row>
-    <row r="65" spans="2:28" ht="33" x14ac:dyDescent="0.3">
+    <row r="65" spans="2:27" ht="33" x14ac:dyDescent="0.3">
       <c r="B65" s="28">
         <v>50</v>
       </c>
@@ -6571,9 +6604,9 @@
       <c r="Z65" s="8" t="s">
         <v>72</v>
       </c>
-      <c r="AA65" s="18"/>
-    </row>
-    <row r="66" spans="2:28" x14ac:dyDescent="0.3">
+      <c r="AA65" s="40"/>
+    </row>
+    <row r="66" spans="2:27" x14ac:dyDescent="0.3">
       <c r="B66" s="28">
         <v>51</v>
       </c>
@@ -6627,24 +6660,24 @@
         <v>41</v>
       </c>
       <c r="T66" s="136"/>
-      <c r="V66" s="123" t="s">
-        <v>21</v>
-      </c>
-      <c r="W66" s="84" t="s">
-        <v>293</v>
-      </c>
-      <c r="X66" s="84" t="s">
-        <v>263</v>
-      </c>
-      <c r="Y66" s="84" t="s">
-        <v>266</v>
-      </c>
-      <c r="Z66" s="84" t="s">
-        <v>41</v>
-      </c>
-      <c r="AA66" s="136"/>
-    </row>
-    <row r="67" spans="2:28" x14ac:dyDescent="0.3">
+      <c r="V66" s="29" t="s">
+        <v>378</v>
+      </c>
+      <c r="W66" s="8" t="s">
+        <v>379</v>
+      </c>
+      <c r="X66" s="8" t="s">
+        <v>72</v>
+      </c>
+      <c r="Y66" s="8" t="s">
+        <v>72</v>
+      </c>
+      <c r="Z66" s="8" t="s">
+        <v>72</v>
+      </c>
+      <c r="AA66" s="40"/>
+    </row>
+    <row r="67" spans="2:27" x14ac:dyDescent="0.3">
       <c r="B67" s="28">
         <v>52</v>
       </c>
@@ -6698,24 +6731,24 @@
         <v>41</v>
       </c>
       <c r="T67" s="136"/>
-      <c r="V67" s="123" t="s">
-        <v>21</v>
-      </c>
-      <c r="W67" s="84" t="s">
-        <v>293</v>
-      </c>
-      <c r="X67" s="84" t="s">
-        <v>262</v>
-      </c>
-      <c r="Y67" s="84" t="s">
-        <v>265</v>
-      </c>
-      <c r="Z67" s="84" t="s">
-        <v>41</v>
-      </c>
-      <c r="AA67" s="136"/>
-    </row>
-    <row r="68" spans="2:28" x14ac:dyDescent="0.3">
+      <c r="V67" s="29" t="s">
+        <v>378</v>
+      </c>
+      <c r="W67" s="8" t="s">
+        <v>379</v>
+      </c>
+      <c r="X67" s="8" t="s">
+        <v>72</v>
+      </c>
+      <c r="Y67" s="8" t="s">
+        <v>72</v>
+      </c>
+      <c r="Z67" s="8" t="s">
+        <v>72</v>
+      </c>
+      <c r="AA67" s="40"/>
+    </row>
+    <row r="68" spans="2:27" x14ac:dyDescent="0.3">
       <c r="B68" s="28">
         <v>53</v>
       </c>
@@ -6776,7 +6809,7 @@
         <v>293</v>
       </c>
       <c r="X68" s="84" t="s">
-        <v>261</v>
+        <v>469</v>
       </c>
       <c r="Y68" s="84" t="s">
         <v>264</v>
@@ -6786,7 +6819,7 @@
       </c>
       <c r="AA68" s="136"/>
     </row>
-    <row r="69" spans="2:28" x14ac:dyDescent="0.3">
+    <row r="69" spans="2:27" x14ac:dyDescent="0.3">
       <c r="B69" s="28">
         <v>54</v>
       </c>
@@ -6853,9 +6886,9 @@
       <c r="Z69" s="8" t="s">
         <v>72</v>
       </c>
-      <c r="AA69" s="18"/>
-    </row>
-    <row r="70" spans="2:28" x14ac:dyDescent="0.3">
+      <c r="AA69" s="40"/>
+    </row>
+    <row r="70" spans="2:27" x14ac:dyDescent="0.3">
       <c r="B70" s="28">
         <v>55</v>
       </c>
@@ -6920,9 +6953,9 @@
       <c r="Z70" s="8" t="s">
         <v>72</v>
       </c>
-      <c r="AA70" s="18"/>
-    </row>
-    <row r="71" spans="2:28" ht="33" x14ac:dyDescent="0.3">
+      <c r="AA70" s="40"/>
+    </row>
+    <row r="71" spans="2:27" ht="33" x14ac:dyDescent="0.3">
       <c r="B71" s="28">
         <v>56</v>
       </c>
@@ -6987,9 +7020,9 @@
       <c r="Z71" s="8" t="s">
         <v>72</v>
       </c>
-      <c r="AA71" s="18"/>
-    </row>
-    <row r="72" spans="2:28" ht="33" x14ac:dyDescent="0.3">
+      <c r="AA71" s="40"/>
+    </row>
+    <row r="72" spans="2:27" ht="33" x14ac:dyDescent="0.3">
       <c r="B72" s="28">
         <v>57</v>
       </c>
@@ -7058,9 +7091,9 @@
       <c r="Z72" s="8" t="s">
         <v>72</v>
       </c>
-      <c r="AA72" s="18"/>
-    </row>
-    <row r="73" spans="2:28" ht="33" x14ac:dyDescent="0.3">
+      <c r="AA72" s="40"/>
+    </row>
+    <row r="73" spans="2:27" ht="33" x14ac:dyDescent="0.3">
       <c r="B73" s="28">
         <v>58</v>
       </c>
@@ -7125,9 +7158,9 @@
       <c r="Z73" s="8" t="s">
         <v>72</v>
       </c>
-      <c r="AA73" s="18"/>
-    </row>
-    <row r="74" spans="2:28" ht="33" x14ac:dyDescent="0.3">
+      <c r="AA73" s="40"/>
+    </row>
+    <row r="74" spans="2:27" ht="33" x14ac:dyDescent="0.3">
       <c r="B74" s="28">
         <v>59</v>
       </c>
@@ -7192,9 +7225,9 @@
       <c r="Z74" s="8" t="s">
         <v>72</v>
       </c>
-      <c r="AA74" s="18"/>
-    </row>
-    <row r="75" spans="2:28" x14ac:dyDescent="0.3">
+      <c r="AA74" s="40"/>
+    </row>
+    <row r="75" spans="2:27" x14ac:dyDescent="0.3">
       <c r="B75" s="30">
         <v>60</v>
       </c>
@@ -7229,15 +7262,15 @@
       <c r="V75" s="30" t="s">
         <v>295</v>
       </c>
-      <c r="W75" s="144"/>
-      <c r="X75" s="144" t="s">
+      <c r="W75" s="157"/>
+      <c r="X75" s="157" t="s">
         <v>295</v>
       </c>
-      <c r="Y75" s="144"/>
-      <c r="Z75" s="144"/>
-      <c r="AA75" s="18"/>
-    </row>
-    <row r="76" spans="2:28" x14ac:dyDescent="0.3">
+      <c r="Y75" s="157"/>
+      <c r="Z75" s="157"/>
+      <c r="AA75" s="42"/>
+    </row>
+    <row r="76" spans="2:27" x14ac:dyDescent="0.3">
       <c r="B76" s="28">
         <v>61</v>
       </c>
@@ -7306,7 +7339,7 @@
         <v>305</v>
       </c>
       <c r="Y76" s="84" t="s">
-        <v>285</v>
+        <v>470</v>
       </c>
       <c r="Z76" s="84" t="s">
         <v>25</v>
@@ -7314,11 +7347,8 @@
       <c r="AA76" s="137" t="s">
         <v>302</v>
       </c>
-      <c r="AB76" s="1" t="s">
-        <v>307</v>
-      </c>
-    </row>
-    <row r="77" spans="2:28" ht="49.5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="77" spans="2:27" ht="49.5" x14ac:dyDescent="0.3">
       <c r="B77" s="28">
         <v>62</v>
       </c>
@@ -7375,27 +7405,24 @@
       <c r="U77" s="1" t="s">
         <v>306</v>
       </c>
-      <c r="V77" s="123" t="s">
-        <v>65</v>
-      </c>
-      <c r="W77" s="84" t="s">
-        <v>49</v>
-      </c>
-      <c r="X77" s="84" t="s">
-        <v>278</v>
-      </c>
-      <c r="Y77" s="84" t="s">
-        <v>285</v>
-      </c>
-      <c r="Z77" s="84" t="s">
-        <v>41</v>
-      </c>
-      <c r="AA77" s="136"/>
-      <c r="AB77" s="1" t="s">
-        <v>306</v>
-      </c>
-    </row>
-    <row r="78" spans="2:28" x14ac:dyDescent="0.3">
+      <c r="V77" s="29" t="s">
+        <v>378</v>
+      </c>
+      <c r="W77" s="8" t="s">
+        <v>379</v>
+      </c>
+      <c r="X77" s="8" t="s">
+        <v>72</v>
+      </c>
+      <c r="Y77" s="8" t="s">
+        <v>72</v>
+      </c>
+      <c r="Z77" s="8" t="s">
+        <v>72</v>
+      </c>
+      <c r="AA77" s="40"/>
+    </row>
+    <row r="78" spans="2:27" x14ac:dyDescent="0.3">
       <c r="B78" s="30">
         <v>63</v>
       </c>
@@ -7424,13 +7451,13 @@
       <c r="S78" s="55"/>
       <c r="T78" s="42"/>
       <c r="V78" s="30"/>
-      <c r="W78" s="144"/>
-      <c r="X78" s="144"/>
-      <c r="Y78" s="144"/>
-      <c r="Z78" s="144"/>
+      <c r="W78" s="157"/>
+      <c r="X78" s="157"/>
+      <c r="Y78" s="157"/>
+      <c r="Z78" s="157"/>
       <c r="AA78" s="42"/>
     </row>
-    <row r="79" spans="2:28" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="79" spans="2:27" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B79" s="31">
         <v>64</v>
       </c>
@@ -7459,10 +7486,10 @@
       <c r="S79" s="56"/>
       <c r="T79" s="70"/>
       <c r="V79" s="31"/>
-      <c r="W79" s="145"/>
-      <c r="X79" s="145"/>
-      <c r="Y79" s="145"/>
-      <c r="Z79" s="145"/>
+      <c r="W79" s="158"/>
+      <c r="X79" s="158"/>
+      <c r="Y79" s="158"/>
+      <c r="Z79" s="158"/>
       <c r="AA79" s="70"/>
     </row>
     <row r="84" spans="5:6" x14ac:dyDescent="0.3">
@@ -7516,16 +7543,16 @@
   </sheetData>
   <autoFilter ref="B15:AB79"/>
   <mergeCells count="28">
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="B4:C4"/>
-    <mergeCell ref="B5:C5"/>
-    <mergeCell ref="B6:C6"/>
-    <mergeCell ref="B7:C7"/>
-    <mergeCell ref="B14:C14"/>
-    <mergeCell ref="I14:J14"/>
-    <mergeCell ref="K14:L14"/>
-    <mergeCell ref="D14:D15"/>
-    <mergeCell ref="G14:H14"/>
+    <mergeCell ref="V14:W14"/>
+    <mergeCell ref="E47:F47"/>
+    <mergeCell ref="E62:F62"/>
+    <mergeCell ref="E63:F63"/>
+    <mergeCell ref="Q14:R14"/>
+    <mergeCell ref="E14:F14"/>
+    <mergeCell ref="E16:F16"/>
+    <mergeCell ref="E22:F22"/>
+    <mergeCell ref="O14:P14"/>
+    <mergeCell ref="X14:AA14"/>
     <mergeCell ref="E78:F78"/>
     <mergeCell ref="E79:F79"/>
     <mergeCell ref="E75:F75"/>
@@ -7534,16 +7561,16 @@
     <mergeCell ref="E33:F33"/>
     <mergeCell ref="E34:F34"/>
     <mergeCell ref="E46:F46"/>
-    <mergeCell ref="V14:W14"/>
-    <mergeCell ref="X14:Y14"/>
-    <mergeCell ref="E47:F47"/>
-    <mergeCell ref="E62:F62"/>
-    <mergeCell ref="E63:F63"/>
-    <mergeCell ref="Q14:R14"/>
-    <mergeCell ref="E14:F14"/>
-    <mergeCell ref="E16:F16"/>
-    <mergeCell ref="E22:F22"/>
-    <mergeCell ref="O14:P14"/>
+    <mergeCell ref="B14:C14"/>
+    <mergeCell ref="I14:J14"/>
+    <mergeCell ref="K14:L14"/>
+    <mergeCell ref="D14:D15"/>
+    <mergeCell ref="G14:H14"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="B4:C4"/>
+    <mergeCell ref="B5:C5"/>
+    <mergeCell ref="B6:C6"/>
+    <mergeCell ref="B7:C7"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -8206,23 +8233,23 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="9" style="158"/>
-    <col min="3" max="3" width="12.75" style="157" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.625" style="157" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.625" style="157" customWidth="1"/>
-    <col min="6" max="6" width="9" style="158"/>
-    <col min="7" max="7" width="11.875" style="157" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="11.375" style="157" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9" style="146"/>
+    <col min="3" max="3" width="12.75" style="145" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.625" style="145" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.625" style="145" customWidth="1"/>
+    <col min="6" max="6" width="9" style="146"/>
+    <col min="7" max="7" width="11.875" style="145" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.375" style="145" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="11.375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:14" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B2" s="158" t="s">
+      <c r="B2" s="146" t="s">
         <v>421</v>
       </c>
     </row>
-    <row r="3" spans="2:14" s="158" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="159" t="s">
+    <row r="3" spans="2:14" s="146" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B3" s="147" t="s">
         <v>459</v>
       </c>
       <c r="C3" s="120" t="s">
@@ -8234,7 +8261,7 @@
       <c r="E3" s="121" t="s">
         <v>464</v>
       </c>
-      <c r="F3" s="159" t="s">
+      <c r="F3" s="147" t="s">
         <v>459</v>
       </c>
       <c r="G3" s="120" t="s">
@@ -8248,23 +8275,23 @@
       </c>
     </row>
     <row r="4" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B4" s="167">
+      <c r="B4" s="155">
         <v>1</v>
       </c>
-      <c r="C4" s="165" t="s">
+      <c r="C4" s="153" t="s">
         <v>384</v>
       </c>
-      <c r="D4" s="160" t="s">
+      <c r="D4" s="148" t="s">
         <v>444</v>
       </c>
-      <c r="E4" s="161"/>
-      <c r="F4" s="167">
+      <c r="E4" s="149"/>
+      <c r="F4" s="155">
         <v>2</v>
       </c>
-      <c r="G4" s="165" t="s">
+      <c r="G4" s="153" t="s">
         <v>385</v>
       </c>
-      <c r="H4" s="160" t="s">
+      <c r="H4" s="148" t="s">
         <v>444</v>
       </c>
       <c r="I4" s="117"/>
@@ -8276,25 +8303,25 @@
       </c>
     </row>
     <row r="5" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B5" s="167">
+      <c r="B5" s="155">
         <v>3</v>
       </c>
-      <c r="C5" s="165" t="s">
+      <c r="C5" s="153" t="s">
         <v>386</v>
       </c>
-      <c r="D5" s="165" t="s">
+      <c r="D5" s="153" t="s">
         <v>445</v>
       </c>
-      <c r="E5" s="164" t="s">
+      <c r="E5" s="152" t="s">
         <v>454</v>
       </c>
-      <c r="F5" s="167">
+      <c r="F5" s="155">
         <v>4</v>
       </c>
-      <c r="G5" s="165" t="s">
+      <c r="G5" s="153" t="s">
         <v>387</v>
       </c>
-      <c r="H5" s="160" t="s">
+      <c r="H5" s="148" t="s">
         <v>444</v>
       </c>
       <c r="I5" s="117"/>
@@ -8306,23 +8333,23 @@
       </c>
     </row>
     <row r="6" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B6" s="167">
+      <c r="B6" s="155">
         <v>5</v>
       </c>
-      <c r="C6" s="165" t="s">
+      <c r="C6" s="153" t="s">
         <v>388</v>
       </c>
-      <c r="D6" s="165" t="s">
+      <c r="D6" s="153" t="s">
         <v>446</v>
       </c>
-      <c r="E6" s="164"/>
-      <c r="F6" s="167">
+      <c r="E6" s="152"/>
+      <c r="F6" s="155">
         <v>6</v>
       </c>
-      <c r="G6" s="165" t="s">
+      <c r="G6" s="153" t="s">
         <v>389</v>
       </c>
-      <c r="H6" s="160" t="s">
+      <c r="H6" s="148" t="s">
         <v>444</v>
       </c>
       <c r="I6" s="117"/>
@@ -8336,23 +8363,23 @@
       </c>
     </row>
     <row r="7" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B7" s="167">
+      <c r="B7" s="155">
         <v>7</v>
       </c>
-      <c r="C7" s="165" t="s">
+      <c r="C7" s="153" t="s">
         <v>390</v>
       </c>
-      <c r="D7" s="165" t="s">
+      <c r="D7" s="153" t="s">
         <v>447</v>
       </c>
-      <c r="E7" s="164"/>
-      <c r="F7" s="167">
+      <c r="E7" s="152"/>
+      <c r="F7" s="155">
         <v>8</v>
       </c>
-      <c r="G7" s="165" t="s">
+      <c r="G7" s="153" t="s">
         <v>392</v>
       </c>
-      <c r="H7" s="160" t="s">
+      <c r="H7" s="148" t="s">
         <v>444</v>
       </c>
       <c r="I7" s="117"/>
@@ -8364,23 +8391,23 @@
       </c>
     </row>
     <row r="8" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B8" s="167">
+      <c r="B8" s="155">
         <v>9</v>
       </c>
-      <c r="C8" s="165" t="s">
+      <c r="C8" s="153" t="s">
         <v>391</v>
       </c>
-      <c r="D8" s="160" t="s">
+      <c r="D8" s="148" t="s">
         <v>444</v>
       </c>
-      <c r="E8" s="161"/>
-      <c r="F8" s="167">
+      <c r="E8" s="149"/>
+      <c r="F8" s="155">
         <v>10</v>
       </c>
-      <c r="G8" s="165" t="s">
+      <c r="G8" s="153" t="s">
         <v>393</v>
       </c>
-      <c r="H8" s="160" t="s">
+      <c r="H8" s="148" t="s">
         <v>444</v>
       </c>
       <c r="I8" s="117"/>
@@ -8394,23 +8421,23 @@
       </c>
     </row>
     <row r="9" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B9" s="167">
+      <c r="B9" s="155">
         <v>11</v>
       </c>
-      <c r="C9" s="165" t="s">
+      <c r="C9" s="153" t="s">
         <v>394</v>
       </c>
-      <c r="D9" s="160" t="s">
+      <c r="D9" s="148" t="s">
         <v>444</v>
       </c>
-      <c r="E9" s="161"/>
-      <c r="F9" s="167">
+      <c r="E9" s="149"/>
+      <c r="F9" s="155">
         <v>12</v>
       </c>
-      <c r="G9" s="165" t="s">
+      <c r="G9" s="153" t="s">
         <v>395</v>
       </c>
-      <c r="H9" s="160" t="s">
+      <c r="H9" s="148" t="s">
         <v>444</v>
       </c>
       <c r="I9" s="117"/>
@@ -8423,23 +8450,23 @@
       </c>
     </row>
     <row r="10" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B10" s="167">
+      <c r="B10" s="155">
         <v>13</v>
       </c>
-      <c r="C10" s="165" t="s">
+      <c r="C10" s="153" t="s">
         <v>396</v>
       </c>
-      <c r="D10" s="160" t="s">
+      <c r="D10" s="148" t="s">
         <v>444</v>
       </c>
-      <c r="E10" s="161"/>
-      <c r="F10" s="167">
+      <c r="E10" s="149"/>
+      <c r="F10" s="155">
         <v>14</v>
       </c>
-      <c r="G10" s="165" t="s">
+      <c r="G10" s="153" t="s">
         <v>397</v>
       </c>
-      <c r="H10" s="160" t="s">
+      <c r="H10" s="148" t="s">
         <v>444</v>
       </c>
       <c r="I10" s="117"/>
@@ -8450,23 +8477,23 @@
       <c r="N10" s="5"/>
     </row>
     <row r="11" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B11" s="167">
+      <c r="B11" s="155">
         <v>15</v>
       </c>
-      <c r="C11" s="165" t="s">
+      <c r="C11" s="153" t="s">
         <v>398</v>
       </c>
-      <c r="D11" s="160" t="s">
+      <c r="D11" s="148" t="s">
         <v>444</v>
       </c>
-      <c r="E11" s="161"/>
-      <c r="F11" s="167">
+      <c r="E11" s="149"/>
+      <c r="F11" s="155">
         <v>16</v>
       </c>
-      <c r="G11" s="165" t="s">
+      <c r="G11" s="153" t="s">
         <v>400</v>
       </c>
-      <c r="H11" s="160" t="s">
+      <c r="H11" s="148" t="s">
         <v>444</v>
       </c>
       <c r="I11" s="117"/>
@@ -8477,23 +8504,23 @@
       <c r="N11" s="5"/>
     </row>
     <row r="12" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B12" s="167">
+      <c r="B12" s="155">
         <v>17</v>
       </c>
-      <c r="C12" s="165" t="s">
+      <c r="C12" s="153" t="s">
         <v>399</v>
       </c>
-      <c r="D12" s="160" t="s">
+      <c r="D12" s="148" t="s">
         <v>444</v>
       </c>
-      <c r="E12" s="161"/>
-      <c r="F12" s="167">
+      <c r="E12" s="149"/>
+      <c r="F12" s="155">
         <v>18</v>
       </c>
-      <c r="G12" s="165" t="s">
+      <c r="G12" s="153" t="s">
         <v>401</v>
       </c>
-      <c r="H12" s="160" t="s">
+      <c r="H12" s="148" t="s">
         <v>444</v>
       </c>
       <c r="I12" s="117"/>
@@ -8501,23 +8528,23 @@
       <c r="N12" s="5"/>
     </row>
     <row r="13" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B13" s="167">
+      <c r="B13" s="155">
         <v>19</v>
       </c>
-      <c r="C13" s="165" t="s">
+      <c r="C13" s="153" t="s">
         <v>402</v>
       </c>
-      <c r="D13" s="165" t="s">
+      <c r="D13" s="153" t="s">
         <v>402</v>
       </c>
-      <c r="E13" s="164"/>
-      <c r="F13" s="167">
+      <c r="E13" s="152"/>
+      <c r="F13" s="155">
         <v>20</v>
       </c>
-      <c r="G13" s="165" t="s">
+      <c r="G13" s="153" t="s">
         <v>403</v>
       </c>
-      <c r="H13" s="165" t="s">
+      <c r="H13" s="153" t="s">
         <v>403</v>
       </c>
       <c r="I13" s="117"/>
@@ -8525,23 +8552,23 @@
       <c r="N13" s="5"/>
     </row>
     <row r="14" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B14" s="167">
+      <c r="B14" s="155">
         <v>21</v>
       </c>
-      <c r="C14" s="165" t="s">
+      <c r="C14" s="153" t="s">
         <v>404</v>
       </c>
-      <c r="D14" s="165" t="s">
+      <c r="D14" s="153" t="s">
         <v>448</v>
       </c>
-      <c r="E14" s="164"/>
-      <c r="F14" s="167">
+      <c r="E14" s="152"/>
+      <c r="F14" s="155">
         <v>22</v>
       </c>
-      <c r="G14" s="165" t="s">
+      <c r="G14" s="153" t="s">
         <v>405</v>
       </c>
-      <c r="H14" s="160" t="s">
+      <c r="H14" s="148" t="s">
         <v>444</v>
       </c>
       <c r="I14" s="117"/>
@@ -8551,23 +8578,23 @@
       <c r="N14" s="5"/>
     </row>
     <row r="15" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B15" s="167">
+      <c r="B15" s="155">
         <v>23</v>
       </c>
-      <c r="C15" s="165" t="s">
+      <c r="C15" s="153" t="s">
         <v>406</v>
       </c>
-      <c r="D15" s="165" t="s">
+      <c r="D15" s="153" t="s">
         <v>448</v>
       </c>
-      <c r="E15" s="164"/>
-      <c r="F15" s="167">
+      <c r="E15" s="152"/>
+      <c r="F15" s="155">
         <v>24</v>
       </c>
-      <c r="G15" s="165" t="s">
+      <c r="G15" s="153" t="s">
         <v>406</v>
       </c>
-      <c r="H15" s="160" t="s">
+      <c r="H15" s="148" t="s">
         <v>444</v>
       </c>
       <c r="I15" s="117"/>
@@ -8577,23 +8604,23 @@
       <c r="N15" s="5"/>
     </row>
     <row r="16" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B16" s="167">
+      <c r="B16" s="155">
         <v>25</v>
       </c>
-      <c r="C16" s="165" t="s">
+      <c r="C16" s="153" t="s">
         <v>407</v>
       </c>
-      <c r="D16" s="160" t="s">
+      <c r="D16" s="148" t="s">
         <v>444</v>
       </c>
-      <c r="E16" s="161"/>
-      <c r="F16" s="167">
+      <c r="E16" s="149"/>
+      <c r="F16" s="155">
         <v>26</v>
       </c>
-      <c r="G16" s="165" t="s">
+      <c r="G16" s="153" t="s">
         <v>414</v>
       </c>
-      <c r="H16" s="160" t="s">
+      <c r="H16" s="148" t="s">
         <v>444</v>
       </c>
       <c r="I16" s="117"/>
@@ -8604,23 +8631,23 @@
       <c r="N16" s="5"/>
     </row>
     <row r="17" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B17" s="167">
+      <c r="B17" s="155">
         <v>27</v>
       </c>
-      <c r="C17" s="165" t="s">
+      <c r="C17" s="153" t="s">
         <v>408</v>
       </c>
-      <c r="D17" s="160" t="s">
+      <c r="D17" s="148" t="s">
         <v>444</v>
       </c>
-      <c r="E17" s="161"/>
-      <c r="F17" s="167">
+      <c r="E17" s="149"/>
+      <c r="F17" s="155">
         <v>28</v>
       </c>
-      <c r="G17" s="165" t="s">
+      <c r="G17" s="153" t="s">
         <v>415</v>
       </c>
-      <c r="H17" s="160" t="s">
+      <c r="H17" s="148" t="s">
         <v>444</v>
       </c>
       <c r="I17" s="117"/>
@@ -8628,23 +8655,23 @@
       <c r="N17" s="5"/>
     </row>
     <row r="18" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B18" s="167">
+      <c r="B18" s="155">
         <v>29</v>
       </c>
-      <c r="C18" s="165" t="s">
+      <c r="C18" s="153" t="s">
         <v>409</v>
       </c>
-      <c r="D18" s="160" t="s">
+      <c r="D18" s="148" t="s">
         <v>444</v>
       </c>
-      <c r="E18" s="161"/>
-      <c r="F18" s="167">
+      <c r="E18" s="149"/>
+      <c r="F18" s="155">
         <v>30</v>
       </c>
-      <c r="G18" s="165" t="s">
+      <c r="G18" s="153" t="s">
         <v>416</v>
       </c>
-      <c r="H18" s="160" t="s">
+      <c r="H18" s="148" t="s">
         <v>444</v>
       </c>
       <c r="I18" s="117"/>
@@ -8652,23 +8679,23 @@
       <c r="N18" s="5"/>
     </row>
     <row r="19" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B19" s="167">
+      <c r="B19" s="155">
         <v>31</v>
       </c>
-      <c r="C19" s="165" t="s">
+      <c r="C19" s="153" t="s">
         <v>410</v>
       </c>
-      <c r="D19" s="160" t="s">
+      <c r="D19" s="148" t="s">
         <v>444</v>
       </c>
-      <c r="E19" s="161"/>
-      <c r="F19" s="167">
+      <c r="E19" s="149"/>
+      <c r="F19" s="155">
         <v>32</v>
       </c>
-      <c r="G19" s="165" t="s">
+      <c r="G19" s="153" t="s">
         <v>417</v>
       </c>
-      <c r="H19" s="160" t="s">
+      <c r="H19" s="148" t="s">
         <v>444</v>
       </c>
       <c r="I19" s="117"/>
@@ -8676,23 +8703,23 @@
       <c r="N19" s="5"/>
     </row>
     <row r="20" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B20" s="167">
+      <c r="B20" s="155">
         <v>33</v>
       </c>
-      <c r="C20" s="165" t="s">
+      <c r="C20" s="153" t="s">
         <v>411</v>
       </c>
-      <c r="D20" s="160" t="s">
+      <c r="D20" s="148" t="s">
         <v>444</v>
       </c>
-      <c r="E20" s="161"/>
-      <c r="F20" s="167">
+      <c r="E20" s="149"/>
+      <c r="F20" s="155">
         <v>34</v>
       </c>
-      <c r="G20" s="165" t="s">
+      <c r="G20" s="153" t="s">
         <v>418</v>
       </c>
-      <c r="H20" s="160" t="s">
+      <c r="H20" s="148" t="s">
         <v>444</v>
       </c>
       <c r="I20" s="117"/>
@@ -8702,23 +8729,23 @@
       <c r="N20" s="5"/>
     </row>
     <row r="21" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B21" s="167">
+      <c r="B21" s="155">
         <v>35</v>
       </c>
-      <c r="C21" s="165" t="s">
+      <c r="C21" s="153" t="s">
         <v>412</v>
       </c>
-      <c r="D21" s="160" t="s">
+      <c r="D21" s="148" t="s">
         <v>444</v>
       </c>
-      <c r="E21" s="161"/>
-      <c r="F21" s="167">
+      <c r="E21" s="149"/>
+      <c r="F21" s="155">
         <v>36</v>
       </c>
-      <c r="G21" s="165" t="s">
+      <c r="G21" s="153" t="s">
         <v>419</v>
       </c>
-      <c r="H21" s="160" t="s">
+      <c r="H21" s="148" t="s">
         <v>444</v>
       </c>
       <c r="I21" s="117"/>
@@ -8728,23 +8755,23 @@
       <c r="N21" s="5"/>
     </row>
     <row r="22" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B22" s="167">
+      <c r="B22" s="155">
         <v>37</v>
       </c>
-      <c r="C22" s="165" t="s">
+      <c r="C22" s="153" t="s">
         <v>413</v>
       </c>
-      <c r="D22" s="160" t="s">
+      <c r="D22" s="148" t="s">
         <v>444</v>
       </c>
-      <c r="E22" s="161"/>
-      <c r="F22" s="167">
+      <c r="E22" s="149"/>
+      <c r="F22" s="155">
         <v>38</v>
       </c>
-      <c r="G22" s="165" t="s">
+      <c r="G22" s="153" t="s">
         <v>420</v>
       </c>
-      <c r="H22" s="160" t="s">
+      <c r="H22" s="148" t="s">
         <v>444</v>
       </c>
       <c r="I22" s="117"/>
@@ -8754,34 +8781,34 @@
       </c>
     </row>
     <row r="23" spans="2:14" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B23" s="168">
+      <c r="B23" s="156">
         <v>39</v>
       </c>
-      <c r="C23" s="166" t="s">
+      <c r="C23" s="154" t="s">
         <v>408</v>
       </c>
-      <c r="D23" s="162" t="s">
+      <c r="D23" s="150" t="s">
         <v>444</v>
       </c>
-      <c r="E23" s="163"/>
-      <c r="F23" s="168">
+      <c r="E23" s="151"/>
+      <c r="F23" s="156">
         <v>40</v>
       </c>
-      <c r="G23" s="166" t="s">
+      <c r="G23" s="154" t="s">
         <v>415</v>
       </c>
-      <c r="H23" s="162" t="s">
+      <c r="H23" s="150" t="s">
         <v>444</v>
       </c>
       <c r="I23" s="119"/>
     </row>
     <row r="25" spans="2:14" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B25" s="158" t="s">
+      <c r="B25" s="146" t="s">
         <v>422</v>
       </c>
     </row>
-    <row r="26" spans="2:14" s="158" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="B26" s="159" t="s">
+    <row r="26" spans="2:14" s="146" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B26" s="147" t="s">
         <v>459</v>
       </c>
       <c r="C26" s="120" t="s">
@@ -8793,7 +8820,7 @@
       <c r="E26" s="121" t="s">
         <v>464</v>
       </c>
-      <c r="F26" s="159" t="s">
+      <c r="F26" s="147" t="s">
         <v>459</v>
       </c>
       <c r="G26" s="120" t="s">
@@ -8807,451 +8834,451 @@
       </c>
     </row>
     <row r="27" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B27" s="167">
+      <c r="B27" s="155">
         <v>1</v>
       </c>
-      <c r="C27" s="165" t="s">
+      <c r="C27" s="153" t="s">
         <v>455</v>
       </c>
-      <c r="D27" s="165" t="s">
+      <c r="D27" s="153" t="s">
         <v>449</v>
       </c>
-      <c r="E27" s="164" t="s">
+      <c r="E27" s="152" t="s">
         <v>460</v>
       </c>
-      <c r="F27" s="167">
+      <c r="F27" s="155">
         <v>2</v>
       </c>
-      <c r="G27" s="165" t="s">
+      <c r="G27" s="153" t="s">
         <v>426</v>
       </c>
-      <c r="H27" s="160" t="s">
+      <c r="H27" s="148" t="s">
         <v>444</v>
       </c>
       <c r="I27" s="117"/>
     </row>
     <row r="28" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B28" s="167">
+      <c r="B28" s="155">
         <v>3</v>
       </c>
-      <c r="C28" s="165" t="s">
+      <c r="C28" s="153" t="s">
         <v>425</v>
       </c>
-      <c r="D28" s="160" t="s">
+      <c r="D28" s="148" t="s">
         <v>444</v>
       </c>
-      <c r="E28" s="161"/>
-      <c r="F28" s="167">
+      <c r="E28" s="149"/>
+      <c r="F28" s="155">
         <v>4</v>
       </c>
-      <c r="G28" s="165" t="s">
+      <c r="G28" s="153" t="s">
         <v>427</v>
       </c>
-      <c r="H28" s="160" t="s">
+      <c r="H28" s="148" t="s">
         <v>444</v>
       </c>
       <c r="I28" s="117"/>
     </row>
     <row r="29" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B29" s="167">
+      <c r="B29" s="155">
         <v>5</v>
       </c>
-      <c r="C29" s="165" t="s">
+      <c r="C29" s="153" t="s">
         <v>423</v>
       </c>
-      <c r="D29" s="160" t="s">
+      <c r="D29" s="148" t="s">
         <v>444</v>
       </c>
-      <c r="E29" s="161"/>
-      <c r="F29" s="167">
+      <c r="E29" s="149"/>
+      <c r="F29" s="155">
         <v>6</v>
       </c>
-      <c r="G29" s="165" t="s">
+      <c r="G29" s="153" t="s">
         <v>428</v>
       </c>
-      <c r="H29" s="160" t="s">
+      <c r="H29" s="148" t="s">
         <v>444</v>
       </c>
       <c r="I29" s="117"/>
     </row>
     <row r="30" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B30" s="167">
+      <c r="B30" s="155">
         <v>7</v>
       </c>
-      <c r="C30" s="165" t="s">
+      <c r="C30" s="153" t="s">
         <v>424</v>
       </c>
-      <c r="D30" s="160" t="s">
+      <c r="D30" s="148" t="s">
         <v>444</v>
       </c>
-      <c r="E30" s="161"/>
-      <c r="F30" s="167">
+      <c r="E30" s="149"/>
+      <c r="F30" s="155">
         <v>8</v>
       </c>
-      <c r="G30" s="165" t="s">
+      <c r="G30" s="153" t="s">
         <v>425</v>
       </c>
-      <c r="H30" s="160" t="s">
+      <c r="H30" s="148" t="s">
         <v>444</v>
       </c>
       <c r="I30" s="117"/>
     </row>
     <row r="31" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B31" s="167">
+      <c r="B31" s="155">
         <v>9</v>
       </c>
-      <c r="C31" s="165" t="s">
+      <c r="C31" s="153" t="s">
         <v>404</v>
       </c>
-      <c r="D31" s="160" t="s">
+      <c r="D31" s="148" t="s">
         <v>444</v>
       </c>
-      <c r="E31" s="161"/>
-      <c r="F31" s="167">
+      <c r="E31" s="149"/>
+      <c r="F31" s="155">
         <v>10</v>
       </c>
-      <c r="G31" s="165" t="s">
+      <c r="G31" s="153" t="s">
         <v>405</v>
       </c>
-      <c r="H31" s="160" t="s">
+      <c r="H31" s="148" t="s">
         <v>444</v>
       </c>
       <c r="I31" s="117"/>
     </row>
     <row r="32" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B32" s="167">
+      <c r="B32" s="155">
         <v>11</v>
       </c>
-      <c r="C32" s="165" t="s">
+      <c r="C32" s="153" t="s">
         <v>429</v>
       </c>
-      <c r="D32" s="160" t="s">
+      <c r="D32" s="148" t="s">
         <v>444</v>
       </c>
-      <c r="E32" s="161"/>
-      <c r="F32" s="167">
+      <c r="E32" s="149"/>
+      <c r="F32" s="155">
         <v>12</v>
       </c>
-      <c r="G32" s="165" t="s">
+      <c r="G32" s="153" t="s">
         <v>438</v>
       </c>
-      <c r="H32" s="160" t="s">
+      <c r="H32" s="148" t="s">
         <v>444</v>
       </c>
       <c r="I32" s="117"/>
     </row>
     <row r="33" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B33" s="167">
+      <c r="B33" s="155">
         <v>13</v>
       </c>
-      <c r="C33" s="165" t="s">
+      <c r="C33" s="153" t="s">
         <v>456</v>
       </c>
-      <c r="D33" s="165" t="s">
+      <c r="D33" s="153" t="s">
         <v>450</v>
       </c>
-      <c r="E33" s="164" t="s">
+      <c r="E33" s="152" t="s">
         <v>461</v>
       </c>
-      <c r="F33" s="167">
+      <c r="F33" s="155">
         <v>14</v>
       </c>
-      <c r="G33" s="165" t="s">
+      <c r="G33" s="153" t="s">
         <v>411</v>
       </c>
-      <c r="H33" s="160" t="s">
+      <c r="H33" s="148" t="s">
         <v>444</v>
       </c>
       <c r="I33" s="117"/>
     </row>
     <row r="34" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B34" s="167">
+      <c r="B34" s="155">
         <v>15</v>
       </c>
-      <c r="C34" s="165" t="s">
+      <c r="C34" s="153" t="s">
         <v>418</v>
       </c>
-      <c r="D34" s="160" t="s">
+      <c r="D34" s="148" t="s">
         <v>444</v>
       </c>
-      <c r="E34" s="161"/>
-      <c r="F34" s="167">
+      <c r="E34" s="149"/>
+      <c r="F34" s="155">
         <v>16</v>
       </c>
-      <c r="G34" s="165" t="s">
+      <c r="G34" s="153" t="s">
         <v>412</v>
       </c>
-      <c r="H34" s="160" t="s">
+      <c r="H34" s="148" t="s">
         <v>444</v>
       </c>
       <c r="I34" s="117"/>
     </row>
     <row r="35" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B35" s="167">
+      <c r="B35" s="155">
         <v>17</v>
       </c>
-      <c r="C35" s="165" t="s">
+      <c r="C35" s="153" t="s">
         <v>427</v>
       </c>
-      <c r="D35" s="160" t="s">
+      <c r="D35" s="148" t="s">
         <v>444</v>
       </c>
-      <c r="E35" s="161"/>
-      <c r="F35" s="167">
+      <c r="E35" s="149"/>
+      <c r="F35" s="155">
         <v>18</v>
       </c>
-      <c r="G35" s="165" t="s">
+      <c r="G35" s="153" t="s">
         <v>428</v>
       </c>
-      <c r="H35" s="160" t="s">
+      <c r="H35" s="148" t="s">
         <v>444</v>
       </c>
       <c r="I35" s="117"/>
     </row>
     <row r="36" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B36" s="167">
+      <c r="B36" s="155">
         <v>19</v>
       </c>
-      <c r="C36" s="165" t="s">
+      <c r="C36" s="153" t="s">
         <v>430</v>
       </c>
-      <c r="D36" s="160" t="s">
+      <c r="D36" s="148" t="s">
         <v>444</v>
       </c>
-      <c r="E36" s="161"/>
-      <c r="F36" s="167">
+      <c r="E36" s="149"/>
+      <c r="F36" s="155">
         <v>20</v>
       </c>
-      <c r="G36" s="165" t="s">
+      <c r="G36" s="153" t="s">
         <v>435</v>
       </c>
-      <c r="H36" s="160" t="s">
+      <c r="H36" s="148" t="s">
         <v>444</v>
       </c>
       <c r="I36" s="117"/>
     </row>
     <row r="37" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B37" s="167">
+      <c r="B37" s="155">
         <v>21</v>
       </c>
-      <c r="C37" s="165" t="s">
+      <c r="C37" s="153" t="s">
         <v>431</v>
       </c>
-      <c r="D37" s="160" t="s">
+      <c r="D37" s="148" t="s">
         <v>444</v>
       </c>
-      <c r="E37" s="161"/>
-      <c r="F37" s="167">
+      <c r="E37" s="149"/>
+      <c r="F37" s="155">
         <v>22</v>
       </c>
-      <c r="G37" s="165" t="s">
+      <c r="G37" s="153" t="s">
         <v>457</v>
       </c>
-      <c r="H37" s="165" t="s">
+      <c r="H37" s="153" t="s">
         <v>462</v>
       </c>
-      <c r="I37" s="164" t="s">
+      <c r="I37" s="152" t="s">
         <v>451</v>
       </c>
     </row>
     <row r="38" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B38" s="167">
+      <c r="B38" s="155">
         <v>23</v>
       </c>
-      <c r="C38" s="165" t="s">
+      <c r="C38" s="153" t="s">
         <v>432</v>
       </c>
-      <c r="D38" s="160" t="s">
+      <c r="D38" s="148" t="s">
         <v>444</v>
       </c>
-      <c r="E38" s="161"/>
-      <c r="F38" s="167">
+      <c r="E38" s="149"/>
+      <c r="F38" s="155">
         <v>24</v>
       </c>
-      <c r="G38" s="165" t="s">
+      <c r="G38" s="153" t="s">
         <v>458</v>
       </c>
-      <c r="H38" s="165" t="s">
+      <c r="H38" s="153" t="s">
         <v>463</v>
       </c>
-      <c r="I38" s="164" t="s">
+      <c r="I38" s="152" t="s">
         <v>452</v>
       </c>
     </row>
     <row r="39" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B39" s="167">
+      <c r="B39" s="155">
         <v>25</v>
       </c>
-      <c r="C39" s="165" t="s">
+      <c r="C39" s="153" t="s">
         <v>430</v>
       </c>
-      <c r="D39" s="160" t="s">
+      <c r="D39" s="148" t="s">
         <v>444</v>
       </c>
-      <c r="E39" s="161"/>
-      <c r="F39" s="167">
+      <c r="E39" s="149"/>
+      <c r="F39" s="155">
         <v>26</v>
       </c>
-      <c r="G39" s="165" t="s">
+      <c r="G39" s="153" t="s">
         <v>431</v>
       </c>
-      <c r="H39" s="160" t="s">
+      <c r="H39" s="148" t="s">
         <v>444</v>
       </c>
       <c r="I39" s="117"/>
     </row>
     <row r="40" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B40" s="167">
+      <c r="B40" s="155">
         <v>27</v>
       </c>
-      <c r="C40" s="165" t="s">
+      <c r="C40" s="153" t="s">
         <v>433</v>
       </c>
-      <c r="D40" s="160" t="s">
+      <c r="D40" s="148" t="s">
         <v>444</v>
       </c>
-      <c r="E40" s="161"/>
-      <c r="F40" s="167">
+      <c r="E40" s="149"/>
+      <c r="F40" s="155">
         <v>28</v>
       </c>
-      <c r="G40" s="165" t="s">
+      <c r="G40" s="153" t="s">
         <v>439</v>
       </c>
-      <c r="H40" s="160" t="s">
+      <c r="H40" s="148" t="s">
         <v>444</v>
       </c>
       <c r="I40" s="117"/>
     </row>
     <row r="41" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B41" s="167">
+      <c r="B41" s="155">
         <v>29</v>
       </c>
-      <c r="C41" s="165" t="s">
+      <c r="C41" s="153" t="s">
         <v>434</v>
       </c>
-      <c r="D41" s="160" t="s">
+      <c r="D41" s="148" t="s">
         <v>444</v>
       </c>
-      <c r="E41" s="161"/>
-      <c r="F41" s="167">
+      <c r="E41" s="149"/>
+      <c r="F41" s="155">
         <v>30</v>
       </c>
-      <c r="G41" s="165" t="s">
+      <c r="G41" s="153" t="s">
         <v>440</v>
       </c>
-      <c r="H41" s="165" t="s">
+      <c r="H41" s="153" t="s">
         <v>440</v>
       </c>
       <c r="I41" s="117"/>
     </row>
     <row r="42" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B42" s="167">
+      <c r="B42" s="155">
         <v>31</v>
       </c>
-      <c r="C42" s="165" t="s">
+      <c r="C42" s="153" t="s">
         <v>435</v>
       </c>
-      <c r="D42" s="160" t="s">
+      <c r="D42" s="148" t="s">
         <v>444</v>
       </c>
-      <c r="E42" s="161"/>
-      <c r="F42" s="167">
+      <c r="E42" s="149"/>
+      <c r="F42" s="155">
         <v>32</v>
       </c>
-      <c r="G42" s="165" t="s">
+      <c r="G42" s="153" t="s">
         <v>419</v>
       </c>
-      <c r="H42" s="165" t="s">
+      <c r="H42" s="153" t="s">
         <v>419</v>
       </c>
       <c r="I42" s="117"/>
     </row>
     <row r="43" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B43" s="167">
+      <c r="B43" s="155">
         <v>33</v>
       </c>
-      <c r="C43" s="165" t="s">
+      <c r="C43" s="153" t="s">
         <v>407</v>
       </c>
-      <c r="D43" s="160" t="s">
+      <c r="D43" s="148" t="s">
         <v>444</v>
       </c>
-      <c r="E43" s="161"/>
-      <c r="F43" s="167">
+      <c r="E43" s="149"/>
+      <c r="F43" s="155">
         <v>34</v>
       </c>
-      <c r="G43" s="165" t="s">
+      <c r="G43" s="153" t="s">
         <v>414</v>
       </c>
-      <c r="H43" s="165" t="s">
+      <c r="H43" s="153" t="s">
         <v>414</v>
       </c>
-      <c r="I43" s="164" t="s">
+      <c r="I43" s="152" t="s">
         <v>453</v>
       </c>
     </row>
     <row r="44" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B44" s="167">
+      <c r="B44" s="155">
         <v>35</v>
       </c>
-      <c r="C44" s="165" t="s">
+      <c r="C44" s="153" t="s">
         <v>413</v>
       </c>
-      <c r="D44" s="160" t="s">
+      <c r="D44" s="148" t="s">
         <v>444</v>
       </c>
-      <c r="E44" s="161"/>
-      <c r="F44" s="167">
+      <c r="E44" s="149"/>
+      <c r="F44" s="155">
         <v>36</v>
       </c>
-      <c r="G44" s="165" t="s">
+      <c r="G44" s="153" t="s">
         <v>420</v>
       </c>
-      <c r="H44" s="160" t="s">
+      <c r="H44" s="148" t="s">
         <v>444</v>
       </c>
       <c r="I44" s="117"/>
     </row>
     <row r="45" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B45" s="167">
+      <c r="B45" s="155">
         <v>37</v>
       </c>
-      <c r="C45" s="165" t="s">
+      <c r="C45" s="153" t="s">
         <v>436</v>
       </c>
-      <c r="D45" s="160" t="s">
+      <c r="D45" s="148" t="s">
         <v>444</v>
       </c>
-      <c r="E45" s="161"/>
-      <c r="F45" s="167">
+      <c r="E45" s="149"/>
+      <c r="F45" s="155">
         <v>38</v>
       </c>
-      <c r="G45" s="165" t="s">
+      <c r="G45" s="153" t="s">
         <v>423</v>
       </c>
-      <c r="H45" s="160" t="s">
+      <c r="H45" s="148" t="s">
         <v>444</v>
       </c>
       <c r="I45" s="117"/>
     </row>
     <row r="46" spans="2:9" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B46" s="168">
+      <c r="B46" s="156">
         <v>39</v>
       </c>
-      <c r="C46" s="166" t="s">
+      <c r="C46" s="154" t="s">
         <v>437</v>
       </c>
-      <c r="D46" s="162" t="s">
+      <c r="D46" s="150" t="s">
         <v>444</v>
       </c>
-      <c r="E46" s="163"/>
-      <c r="F46" s="168">
+      <c r="E46" s="151"/>
+      <c r="F46" s="156">
         <v>40</v>
       </c>
-      <c r="G46" s="166" t="s">
+      <c r="G46" s="154" t="s">
         <v>441</v>
       </c>
-      <c r="H46" s="162" t="s">
+      <c r="H46" s="150" t="s">
         <v>444</v>
       </c>
       <c r="I46" s="119"/>

</xml_diff>

<commit_message>
SW - F/W femto source 추가
</commit_message>
<xml_diff>
--- a/MCU PCB/Plasma_LF_MCU_PinMap_20180117.xlsx
+++ b/MCU PCB/Plasma_LF_MCU_PinMap_20180117.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12975" activeTab="2"/>
@@ -14,7 +14,7 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Pin-map'!$B$15:$AB$79</definedName>
   </definedNames>
-  <calcPr calcId="144525"/>
+  <calcPr calcId="152511" calcMode="manual"/>
 </workbook>
 </file>
 
@@ -2783,6 +2783,84 @@
     <xf numFmtId="0" fontId="6" fillId="3" borderId="6" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="12" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="6" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="4" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="11" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="11" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -2799,84 +2877,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="11" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="11" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="12" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="6" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="4" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -2940,7 +2940,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -2975,7 +2975,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -3247,10 +3247,10 @@
       <c r="X2" s="1"/>
     </row>
     <row r="3" spans="2:27" x14ac:dyDescent="0.3">
-      <c r="B3" s="166" t="s">
+      <c r="B3" s="192" t="s">
         <v>3</v>
       </c>
-      <c r="C3" s="167"/>
+      <c r="C3" s="193"/>
       <c r="D3" s="2">
         <v>128</v>
       </c>
@@ -3278,10 +3278,10 @@
       </c>
     </row>
     <row r="4" spans="2:27" x14ac:dyDescent="0.3">
-      <c r="B4" s="168" t="s">
+      <c r="B4" s="194" t="s">
         <v>5</v>
       </c>
-      <c r="C4" s="169"/>
+      <c r="C4" s="195"/>
       <c r="D4" s="3">
         <v>16</v>
       </c>
@@ -3311,10 +3311,10 @@
       </c>
     </row>
     <row r="5" spans="2:27" x14ac:dyDescent="0.3">
-      <c r="B5" s="168" t="s">
+      <c r="B5" s="194" t="s">
         <v>6</v>
       </c>
-      <c r="C5" s="169"/>
+      <c r="C5" s="195"/>
       <c r="D5" s="3">
         <v>48</v>
       </c>
@@ -3346,10 +3346,10 @@
       </c>
     </row>
     <row r="6" spans="2:27" x14ac:dyDescent="0.3">
-      <c r="B6" s="168" t="s">
+      <c r="B6" s="194" t="s">
         <v>9</v>
       </c>
-      <c r="C6" s="169"/>
+      <c r="C6" s="195"/>
       <c r="D6" s="3" t="s">
         <v>10</v>
       </c>
@@ -3373,10 +3373,10 @@
       <c r="X6" s="18"/>
     </row>
     <row r="7" spans="2:27" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B7" s="170" t="s">
+      <c r="B7" s="196" t="s">
         <v>12</v>
       </c>
-      <c r="C7" s="171"/>
+      <c r="C7" s="197"/>
       <c r="D7" s="4" t="s">
         <v>13</v>
       </c>
@@ -3495,45 +3495,45 @@
     </row>
     <row r="13" spans="2:27" ht="17.25" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="14" spans="2:27" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B14" s="172" t="s">
+      <c r="B14" s="189" t="s">
         <v>178</v>
       </c>
-      <c r="C14" s="173"/>
-      <c r="D14" s="173" t="s">
+      <c r="C14" s="185"/>
+      <c r="D14" s="185" t="s">
         <v>163</v>
       </c>
-      <c r="E14" s="173" t="s">
+      <c r="E14" s="185" t="s">
         <v>165</v>
       </c>
-      <c r="F14" s="185"/>
-      <c r="G14" s="174" t="s">
+      <c r="F14" s="186"/>
+      <c r="G14" s="176" t="s">
         <v>14</v>
       </c>
-      <c r="H14" s="175"/>
-      <c r="I14" s="174" t="s">
+      <c r="H14" s="190"/>
+      <c r="I14" s="176" t="s">
         <v>311</v>
       </c>
-      <c r="J14" s="175"/>
-      <c r="K14" s="174" t="s">
+      <c r="J14" s="190"/>
+      <c r="K14" s="176" t="s">
         <v>312</v>
       </c>
-      <c r="L14" s="176"/>
+      <c r="L14" s="177"/>
       <c r="M14" s="23"/>
       <c r="N14" s="37"/>
-      <c r="O14" s="174" t="s">
+      <c r="O14" s="176" t="s">
         <v>14</v>
       </c>
-      <c r="P14" s="176"/>
-      <c r="Q14" s="176" t="s">
+      <c r="P14" s="177"/>
+      <c r="Q14" s="177" t="s">
         <v>162</v>
       </c>
-      <c r="R14" s="176"/>
+      <c r="R14" s="177"/>
       <c r="S14" s="56"/>
       <c r="T14" s="35"/>
-      <c r="V14" s="174" t="s">
+      <c r="V14" s="176" t="s">
         <v>14</v>
       </c>
-      <c r="W14" s="176"/>
+      <c r="W14" s="177"/>
       <c r="X14" s="178" t="s">
         <v>383</v>
       </c>
@@ -3548,7 +3548,7 @@
       <c r="C15" s="15" t="s">
         <v>180</v>
       </c>
-      <c r="D15" s="177"/>
+      <c r="D15" s="191"/>
       <c r="E15" s="15" t="s">
         <v>248</v>
       </c>
@@ -3626,10 +3626,10 @@
       <c r="D16" s="21" t="s">
         <v>164</v>
       </c>
-      <c r="E16" s="186" t="s">
+      <c r="E16" s="187" t="s">
         <v>176</v>
       </c>
-      <c r="F16" s="187"/>
+      <c r="F16" s="188"/>
       <c r="G16" s="50"/>
       <c r="H16" s="69"/>
       <c r="I16" s="79"/>
@@ -3721,19 +3721,19 @@
       <c r="AA17" s="39"/>
     </row>
     <row r="18" spans="2:27" x14ac:dyDescent="0.3">
-      <c r="B18" s="196">
+      <c r="B18" s="172">
         <v>3</v>
       </c>
-      <c r="C18" s="197">
+      <c r="C18" s="173">
         <v>3</v>
       </c>
-      <c r="D18" s="197" t="s">
+      <c r="D18" s="173" t="s">
         <v>150</v>
       </c>
       <c r="E18" s="8" t="s">
         <v>181</v>
       </c>
-      <c r="F18" s="190" t="s">
+      <c r="F18" s="168" t="s">
         <v>166</v>
       </c>
       <c r="G18" s="64"/>
@@ -3780,19 +3780,19 @@
       <c r="AA18" s="159"/>
     </row>
     <row r="19" spans="2:27" x14ac:dyDescent="0.3">
-      <c r="B19" s="196">
+      <c r="B19" s="172">
         <v>4</v>
       </c>
-      <c r="C19" s="197">
+      <c r="C19" s="173">
         <v>4</v>
       </c>
-      <c r="D19" s="197" t="s">
+      <c r="D19" s="173" t="s">
         <v>151</v>
       </c>
       <c r="E19" s="8" t="s">
         <v>181</v>
       </c>
-      <c r="F19" s="190" t="s">
+      <c r="F19" s="168" t="s">
         <v>167</v>
       </c>
       <c r="G19" s="64"/>
@@ -3839,19 +3839,19 @@
       <c r="AA19" s="159"/>
     </row>
     <row r="20" spans="2:27" x14ac:dyDescent="0.3">
-      <c r="B20" s="196">
+      <c r="B20" s="172">
         <v>5</v>
       </c>
-      <c r="C20" s="197">
+      <c r="C20" s="173">
         <v>5</v>
       </c>
-      <c r="D20" s="197" t="s">
+      <c r="D20" s="173" t="s">
         <v>168</v>
       </c>
       <c r="E20" s="13" t="s">
         <v>172</v>
       </c>
-      <c r="F20" s="190" t="s">
+      <c r="F20" s="168" t="s">
         <v>171</v>
       </c>
       <c r="G20" s="64"/>
@@ -3896,19 +3896,19 @@
       <c r="AA20" s="159"/>
     </row>
     <row r="21" spans="2:27" x14ac:dyDescent="0.3">
-      <c r="B21" s="196">
+      <c r="B21" s="172">
         <v>6</v>
       </c>
-      <c r="C21" s="197">
+      <c r="C21" s="173">
         <v>6</v>
       </c>
-      <c r="D21" s="197" t="s">
+      <c r="D21" s="173" t="s">
         <v>169</v>
       </c>
       <c r="E21" s="13" t="s">
         <v>173</v>
       </c>
-      <c r="F21" s="190" t="s">
+      <c r="F21" s="168" t="s">
         <v>175</v>
       </c>
       <c r="G21" s="64"/>
@@ -3962,13 +3962,13 @@
       <c r="D22" s="98" t="s">
         <v>170</v>
       </c>
-      <c r="E22" s="192" t="s">
+      <c r="E22" s="174" t="s">
         <v>177</v>
       </c>
-      <c r="F22" s="193"/>
+      <c r="F22" s="175"/>
       <c r="G22" s="75"/>
       <c r="H22" s="103"/>
-      <c r="I22" s="194"/>
+      <c r="I22" s="170"/>
       <c r="J22" s="103"/>
       <c r="K22" s="75"/>
       <c r="L22" s="104"/>
@@ -3990,7 +3990,7 @@
         <v>257</v>
       </c>
       <c r="T22" s="103"/>
-      <c r="U22" s="195"/>
+      <c r="U22" s="171"/>
       <c r="V22" s="100" t="s">
         <v>170</v>
       </c>
@@ -4080,7 +4080,7 @@
       <c r="AA23" s="39"/>
     </row>
     <row r="24" spans="2:27" x14ac:dyDescent="0.3">
-      <c r="B24" s="188">
+      <c r="B24" s="166">
         <v>9</v>
       </c>
       <c r="C24" s="8" t="s">
@@ -4151,7 +4151,7 @@
       <c r="AA24" s="81"/>
     </row>
     <row r="25" spans="2:27" x14ac:dyDescent="0.3">
-      <c r="B25" s="188">
+      <c r="B25" s="166">
         <v>10</v>
       </c>
       <c r="C25" s="8" t="s">
@@ -4222,7 +4222,7 @@
       <c r="AA25" s="81"/>
     </row>
     <row r="26" spans="2:27" x14ac:dyDescent="0.3">
-      <c r="B26" s="188">
+      <c r="B26" s="166">
         <v>11</v>
       </c>
       <c r="C26" s="8" t="s">
@@ -4410,7 +4410,7 @@
       <c r="AA29" s="39"/>
     </row>
     <row r="30" spans="2:27" ht="33" x14ac:dyDescent="0.3">
-      <c r="B30" s="188">
+      <c r="B30" s="166">
         <v>15</v>
       </c>
       <c r="C30" s="42">
@@ -4471,7 +4471,7 @@
       </c>
     </row>
     <row r="31" spans="2:27" x14ac:dyDescent="0.3">
-      <c r="B31" s="188">
+      <c r="B31" s="166">
         <v>16</v>
       </c>
       <c r="C31" s="42">
@@ -4661,7 +4661,7 @@
       <c r="AA34" s="41"/>
     </row>
     <row r="35" spans="2:28" ht="33" x14ac:dyDescent="0.3">
-      <c r="B35" s="188">
+      <c r="B35" s="166">
         <v>20</v>
       </c>
       <c r="C35" s="13">
@@ -4732,7 +4732,7 @@
       <c r="AA35" s="134"/>
     </row>
     <row r="36" spans="2:28" x14ac:dyDescent="0.3">
-      <c r="B36" s="188">
+      <c r="B36" s="166">
         <v>21</v>
       </c>
       <c r="C36" s="13">
@@ -4803,7 +4803,7 @@
       <c r="AA36" s="134"/>
     </row>
     <row r="37" spans="2:28" ht="49.5" x14ac:dyDescent="0.3">
-      <c r="B37" s="188">
+      <c r="B37" s="166">
         <v>22</v>
       </c>
       <c r="C37" s="13">
@@ -6062,7 +6062,7 @@
       <c r="AA55" s="39"/>
     </row>
     <row r="56" spans="2:27" ht="33" x14ac:dyDescent="0.3">
-      <c r="B56" s="189">
+      <c r="B56" s="167">
         <v>41</v>
       </c>
       <c r="C56" s="13">
@@ -6074,7 +6074,7 @@
       <c r="E56" s="83" t="s">
         <v>282</v>
       </c>
-      <c r="F56" s="191" t="s">
+      <c r="F56" s="169" t="s">
         <v>181</v>
       </c>
       <c r="G56" s="64"/>
@@ -6253,7 +6253,7 @@
       <c r="AA58" s="94"/>
     </row>
     <row r="59" spans="2:27" ht="33" x14ac:dyDescent="0.3">
-      <c r="B59" s="189">
+      <c r="B59" s="167">
         <v>44</v>
       </c>
       <c r="C59" s="13">
@@ -7222,7 +7222,7 @@
       <c r="AA73" s="39"/>
     </row>
     <row r="74" spans="2:27" ht="33" x14ac:dyDescent="0.3">
-      <c r="B74" s="188">
+      <c r="B74" s="166">
         <v>59</v>
       </c>
       <c r="C74" s="13">
@@ -7332,7 +7332,7 @@
       <c r="AA75" s="41"/>
     </row>
     <row r="76" spans="2:27" x14ac:dyDescent="0.3">
-      <c r="B76" s="188">
+      <c r="B76" s="166">
         <v>61</v>
       </c>
       <c r="C76" s="13">
@@ -7604,6 +7604,18 @@
   </sheetData>
   <autoFilter ref="B15:AB79"/>
   <mergeCells count="28">
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="B4:C4"/>
+    <mergeCell ref="B5:C5"/>
+    <mergeCell ref="B6:C6"/>
+    <mergeCell ref="B7:C7"/>
+    <mergeCell ref="E14:F14"/>
+    <mergeCell ref="E16:F16"/>
+    <mergeCell ref="B14:C14"/>
+    <mergeCell ref="I14:J14"/>
+    <mergeCell ref="K14:L14"/>
+    <mergeCell ref="D14:D15"/>
+    <mergeCell ref="G14:H14"/>
     <mergeCell ref="E22:F22"/>
     <mergeCell ref="O14:P14"/>
     <mergeCell ref="X14:AA14"/>
@@ -7620,18 +7632,6 @@
     <mergeCell ref="E62:F62"/>
     <mergeCell ref="E63:F63"/>
     <mergeCell ref="Q14:R14"/>
-    <mergeCell ref="E14:F14"/>
-    <mergeCell ref="E16:F16"/>
-    <mergeCell ref="B14:C14"/>
-    <mergeCell ref="I14:J14"/>
-    <mergeCell ref="K14:L14"/>
-    <mergeCell ref="D14:D15"/>
-    <mergeCell ref="G14:H14"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="B4:C4"/>
-    <mergeCell ref="B5:C5"/>
-    <mergeCell ref="B6:C6"/>
-    <mergeCell ref="B7:C7"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -8289,7 +8289,7 @@
   <dimension ref="B2:N46"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M26" sqref="M26"/>
+      <selection activeCell="Q20" sqref="Q20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>

</xml_diff>